<commit_message>
add stacked bar charts
</commit_message>
<xml_diff>
--- a/survey analysis.xlsx
+++ b/survey analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Thesis2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDE8D8C-CDCB-4BDC-9629-F812D74DF55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B2795C-241F-41DC-A888-1A9A44B65415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37665" yWindow="-16665" windowWidth="28440" windowHeight="11820" tabRatio="705" firstSheet="2" activeTab="10" xr2:uid="{CF2921A5-C80B-4877-A0CE-2F57B984B9AC}"/>
+    <workbookView xWindow="-23520" yWindow="-16665" windowWidth="28440" windowHeight="11820" tabRatio="705" firstSheet="2" activeTab="10" xr2:uid="{CF2921A5-C80B-4877-A0CE-2F57B984B9AC}"/>
   </bookViews>
   <sheets>
     <sheet name="deliveries" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId13"/>
-    <pivotCache cacheId="57" r:id="rId14"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
+    <pivotCache cacheId="1" r:id="rId14"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1069,10 +1069,10 @@
     <t>circuit</t>
   </si>
   <si>
-    <t>TT First</t>
-  </si>
-  <si>
-    <t>Circuit First</t>
+    <t>circuit first</t>
+  </si>
+  <si>
+    <t>tt first</t>
   </si>
 </sst>
 </file>
@@ -5600,204 +5600,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9EB97D2-B220-420F-9482-6B2082BF4693}" name="PivotTable3" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I9:J25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="44">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="31"/>
-    <field x="27"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="5" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Respondent ID" fld="0" subtotal="count" baseField="9" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{349D25D2-486B-45F2-8B43-2C24FC525FFD}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{349D25D2-486B-45F2-8B43-2C24FC525FFD}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E11:F16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="29">
     <pivotField dataField="1" showAll="0"/>
@@ -5894,8 +5697,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5624DE0F-B479-4E43-A407-7F4A6D86F76C}" name="PivotTable1" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5624DE0F-B479-4E43-A407-7F4A6D86F76C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="44">
     <pivotField dataField="1" showAll="0"/>
@@ -6119,6 +5922,203 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Respondent ID" fld="0" subtotal="count" baseField="6" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9EB97D2-B220-420F-9482-6B2082BF4693}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I9:J25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="44">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="31"/>
+    <field x="27"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="5" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Respondent ID" fld="0" subtotal="count" baseField="9" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -6817,10 +6817,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7F3328-AE59-4804-B9D0-19F41318D13C}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="K15" sqref="K15:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6833,7 +6833,7 @@
     <col min="10" max="10" width="37.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>315</v>
@@ -6859,7 +6859,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>311</v>
       </c>
@@ -6886,15 +6886,27 @@
         <v>5</v>
       </c>
       <c r="I2" s="7" t="str">
-        <f>"'"&amp;A2 &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A2," ","_") &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
         <v>'total' : [0,-9,-2,14,5],</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>"'" &amp; A2 &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A2," ","_")  &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
         <v>'total_pct' : [0,-0.3,-0.07,0.47,0.17],</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="7" t="str">
+        <f>IF(ISBLANK(A2),K3,K3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"_pct[xx]]")</f>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx],df.total_pct[xx]]</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>IF(ISBLANK(A2),L3,L3&amp;",'"&amp; A2 &amp;"']")</f>
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner','academic','total']</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>IF(ISBLANK(A2),M3,M3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"[xx]]")</f>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx],df.total[xx]]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -6905,8 +6917,20 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K13" si="1">IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="shared" ref="L3:L13" si="2">IF(ISBLANK(A3),L4,L4&amp;",'"&amp; A3 &amp;"'")</f>
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f t="shared" ref="M3:M13" si="3">IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>312</v>
       </c>
@@ -6933,15 +6957,27 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A4," ","_") &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [0,-5,-1,3,1],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J4:J13" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A4," ","_")  &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [0,-0.5,-0.1,0.3,0.1],</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>313</v>
       </c>
@@ -6968,15 +7004,27 @@
         <v>4</v>
       </c>
       <c r="I5" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A5," ","_") &amp; "' : [" &amp; (F5*-1) &amp; "," &amp; (E5*-1) &amp; "," &amp;(D5*-1)&amp; "," &amp; G5 &amp; "," &amp; H5 &amp; "],"</f>
+        <v>'practicioner' : [0,-4,-1,11,4],</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A5," ","_")  &amp; "_pct' : [" &amp; ROUND(((F5/B5)*-1),2) &amp; "," &amp; ROUND(((E5/B5)*-1),2) &amp; "," &amp; ROUND(((D5/B5)*-1),2)  &amp; "," &amp; ROUND((G5/B5),2) &amp; "," &amp; ROUND((H5/B5),2) &amp; "],"</f>
+        <v>'practicioner_pct' : [0,-0.2,-0.05,0.55,0.2],</v>
+      </c>
+      <c r="K5" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'practicioner' : [0,-4,-1,11,4],</v>
-      </c>
-      <c r="J5" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'practicioner_pct' : [0,-0.2,-0.05,0.55,0.2],</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner'</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -6985,25 +7033,37 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="3">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="4">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>317</v>
       </c>
@@ -7030,15 +7090,27 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7" si="5">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <v>'expert' : [0,-2,0,6,1],</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A7," ","_")  &amp; "_pct' : [" &amp; ROUND(((F7/B7)*-1),2) &amp; "," &amp; ROUND(((E7/B7)*-1),2) &amp; "," &amp; ROUND(((D7/B7)*-1),2)  &amp; "," &amp; ROUND((G7/B7),2) &amp; "," &amp; ROUND((H7/B7),2) &amp; "],"</f>
+        <v>'expert_pct' : [0,-0.22,0,0.67,0.11],</v>
+      </c>
+      <c r="K7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'expert' : [0,-2,0,6,1],</v>
-      </c>
-      <c r="J7" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L7" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'expert_pct' : [0,-0.22,0,0.67,0.11],</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>318</v>
       </c>
@@ -7065,15 +7137,27 @@
         <v>4</v>
       </c>
       <c r="I8" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A8," ","_") &amp; "' : [" &amp; (F8*-1) &amp; "," &amp; (E8*-1) &amp; "," &amp;(D8*-1)&amp; "," &amp; G8 &amp; "," &amp; H8 &amp; "],"</f>
+        <v>'senior' : [0,-5,-2,5,4],</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A8," ","_")  &amp; "_pct' : [" &amp; ROUND(((F8/B8)*-1),2) &amp; "," &amp; ROUND(((E8/B8)*-1),2) &amp; "," &amp; ROUND(((D8/B8)*-1),2)  &amp; "," &amp; ROUND((G8/B8),2) &amp; "," &amp; ROUND((H8/B8),2) &amp; "],"</f>
+        <v>'senior_pct' : [0,-0.31,-0.13,0.31,0.25],</v>
+      </c>
+      <c r="K8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'senior' : [0,-5,-2,5,4],</v>
-      </c>
-      <c r="J8" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
+      </c>
+      <c r="L8" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'senior_pct' : [0,-0.31,-0.13,0.31,0.25],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice','senior'</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>319</v>
       </c>
@@ -7100,15 +7184,27 @@
         <v>0</v>
       </c>
       <c r="I9" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A9," ","_") &amp; "' : [" &amp; (F9*-1) &amp; "," &amp; (E9*-1) &amp; "," &amp;(D9*-1)&amp; "," &amp; G9 &amp; "," &amp; H9 &amp; "],"</f>
+        <v>'novice' : [0,-2,0,3,0],</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A9," ","_")  &amp; "_pct' : [" &amp; ROUND(((F9/B9)*-1),2) &amp; "," &amp; ROUND(((E9/B9)*-1),2) &amp; "," &amp; ROUND(((D9/B9)*-1),2)  &amp; "," &amp; ROUND((G9/B9),2) &amp; "," &amp; ROUND((H9/B9),2) &amp; "],"</f>
+        <v>'novice_pct' : [0,-0.4,0,0.6,0],</v>
+      </c>
+      <c r="K9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'novice' : [0,-2,0,3,0],</v>
-      </c>
-      <c r="J9" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
+      </c>
+      <c r="L9" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'novice_pct' : [0,-0.4,0,0.6,0],</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice'</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -7117,25 +7213,37 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="b">
-        <f t="shared" ref="E10:H10" si="4">SUM(E7:E9)=E2</f>
+        <f t="shared" ref="E10:H10" si="6">SUM(E7:E9)=E2</f>
         <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first','past','current'</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
@@ -7162,15 +7270,27 @@
         <v>2</v>
       </c>
       <c r="I11" s="7" t="str">
+        <f t="shared" ref="I11" si="7">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <v>'current' : [0,-2,-1,7,2],</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A11," ","_")  &amp; "_pct' : [" &amp; ROUND(((F11/B11)*-1),2) &amp; "," &amp; ROUND(((E11/B11)*-1),2) &amp; "," &amp; ROUND(((D11/B11)*-1),2)  &amp; "," &amp; ROUND((G11/B11),2) &amp; "," &amp; ROUND((H11/B11),2) &amp; "],"</f>
+        <v>'current_pct' : [0,-0.17,-0.08,0.58,0.17],</v>
+      </c>
+      <c r="K11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'current' : [0,-2,-1,7,2],</v>
-      </c>
-      <c r="J11" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'current_pct' : [0,-0.17,-0.08,0.58,0.17],</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current'</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -7197,15 +7317,27 @@
         <v>3</v>
       </c>
       <c r="I12" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A12," ","_") &amp; "' : [" &amp; (F12*-1) &amp; "," &amp; (E12*-1) &amp; "," &amp;(D12*-1)&amp; "," &amp; G12 &amp; "," &amp; H12 &amp; "],"</f>
+        <v>'past' : [0,-7,-1,7,3],</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A12," ","_")  &amp; "_pct' : [" &amp; ROUND(((F12/B12)*-1),2) &amp; "," &amp; ROUND(((E12/B12)*-1),2) &amp; "," &amp; ROUND(((D12/B12)*-1),2)  &amp; "," &amp; ROUND((G12/B12),2) &amp; "," &amp; ROUND((H12/B12),2) &amp; "],"</f>
+        <v>'past_pct' : [0,-0.39,-0.06,0.39,0.17],</v>
+      </c>
+      <c r="K12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'past' : [0,-7,-1,7,3],</v>
-      </c>
-      <c r="J12" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx]</v>
+      </c>
+      <c r="L12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'past_pct' : [0,-0.39,-0.06,0.39,0.17],</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past'</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -7214,27 +7346,39 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="5">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="8">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx]</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first'</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B14" s="7">
         <v>14</v>
@@ -7259,17 +7403,29 @@
         <v>2</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14:I15" si="6">"'"&amp;A14 &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
-        <v>'TT First' : [0,-5,0,7,2],</v>
+        <f t="shared" ref="I14" si="9">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <v>'tt_first' : [0,-5,0,7,2],</v>
       </c>
       <c r="J14" s="7" t="str">
-        <f t="shared" ref="J14:J15" si="7">"'" &amp; A14 &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
-        <v>'TT First_pct' : [0,-0.36,0,0.5,0.14],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A14," ","_")  &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
+        <v>'tt_first_pct' : [0,-0.36,0,0.5,0.14],</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f>IF(ISBLANK(A14),K15,K15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx]</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" ref="L14" si="10">IF(ISBLANK(A14),L15,L15&amp;",'"&amp; A14 &amp;"'")</f>
+        <v>['circuit first','tt first'</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f>IF(ISBLANK(A14),M15,M15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"[xx]")</f>
+        <v>[df.circuit_first[xx],df.tt_first[xx]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B15" s="7">
         <v>16</v>
@@ -7294,15 +7450,27 @@
         <v>3</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>'Circuit First' : [0,-4,-2,7,3],</v>
+        <f>"'"&amp;SUBSTITUTE(A15," ","_") &amp; "' : [" &amp; (F15*-1) &amp; "," &amp; (E15*-1) &amp; "," &amp;(D15*-1)&amp; "," &amp; G15 &amp; "," &amp; H15 &amp; "],"</f>
+        <v>'circuit_first' : [0,-4,-2,7,3],</v>
       </c>
       <c r="J15" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>'Circuit First_pct' : [0,-0.25,-0.13,0.44,0.19],</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A15," ","_")  &amp; "_pct' : [" &amp; ROUND(((F15/B15)*-1),2) &amp; "," &amp; ROUND(((E15/B15)*-1),2) &amp; "," &amp; ROUND(((D15/B15)*-1),2)  &amp; "," &amp; ROUND((G15/B15),2) &amp; "," &amp; ROUND((H15/B15),2) &amp; "],"</f>
+        <v>'circuit_first_pct' : [0,-0.25,-0.13,0.44,0.19],</v>
+      </c>
+      <c r="K15" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A15," ","_") &amp;"_pct[xx]"</f>
+        <v>[df.circuit_first_pct[xx]</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f>"['"&amp; A15&amp;"'"</f>
+        <v>['circuit first'</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A15," ","_") &amp;"[xx]"</f>
+        <v>[df.circuit_first[xx]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -7311,23 +7479,43 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="b">
-        <f t="shared" ref="E16:H16" si="8">SUM(E14:E15)=E$2</f>
+        <f t="shared" ref="E16:H16" si="11">SUM(E14:E15)=E$2</f>
         <v>1</v>
       </c>
       <c r="F16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="G16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="H16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7336,10 +7524,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E89FD6-A5B3-49FA-9795-07F4C25BE734}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7353,7 +7541,7 @@
     <col min="11" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="7" t="s">
         <v>315</v>
       </c>
@@ -7376,7 +7564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>311</v>
       </c>
@@ -7403,15 +7591,41 @@
         <v>2</v>
       </c>
       <c r="I2" s="7" t="str">
-        <f>"'"&amp;A2 &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A2," ","_") &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
         <v>'total' : [-4,-7,-3,14,2],</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>"'" &amp; A2 &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A2," ","_")  &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
         <v>'total_pct' : [-0.13,-0.23,-0.1,0.47,0.07],</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="7" t="str">
+        <f>IF(ISBLANK(A2),K3,K3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"_pct[xx]]")</f>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx],df.total_pct[xx]]</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>IF(ISBLANK(A2),L3,L3&amp;",'"&amp; A2 &amp;"']")</f>
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner','academic','total']</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>IF(ISBLANK(A2),M3,M3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"[xx]]")</f>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx],df.total[xx]]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K13" si="1">IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="shared" ref="L3:L14" si="2">IF(ISBLANK(A3),L4,L4&amp;",'"&amp; A3 &amp;"'")</f>
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f t="shared" ref="M3:M13" si="3">IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>312</v>
       </c>
@@ -7438,15 +7652,27 @@
         <v>0</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A4," ","_") &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [-1,-1,-1,7,0],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J4:J13" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A4," ","_")  &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [-0.1,-0.1,-0.1,0.7,0],</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>313</v>
       </c>
@@ -7473,37 +7699,61 @@
         <v>2</v>
       </c>
       <c r="I5" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A5," ","_") &amp; "' : [" &amp; (F5*-1) &amp; "," &amp; (E5*-1) &amp; "," &amp;(D5*-1)&amp; "," &amp; G5 &amp; "," &amp; H5 &amp; "],"</f>
+        <v>'practicioner' : [-3,-6,-2,7,2],</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A5," ","_")  &amp; "_pct' : [" &amp; ROUND(((F5/B5)*-1),2) &amp; "," &amp; ROUND(((E5/B5)*-1),2) &amp; "," &amp; ROUND(((D5/B5)*-1),2)  &amp; "," &amp; ROUND((G5/B5),2) &amp; "," &amp; ROUND((H5/B5),2) &amp; "],"</f>
+        <v>'practicioner_pct' : [-0.15,-0.3,-0.1,0.35,0.1],</v>
+      </c>
+      <c r="K5" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'practicioner' : [-3,-6,-2,7,2],</v>
-      </c>
-      <c r="J5" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'practicioner_pct' : [-0.15,-0.3,-0.1,0.35,0.1],</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice','senior','expert','practicioner'</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D6" s="7" t="b">
         <f>SUM(D4:D5)=D2</f>
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="3">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="4">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M6" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G6" s="7" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H6" s="7" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>317</v>
       </c>
@@ -7530,15 +7780,27 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7" si="5">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <v>'expert' : [-3,-1,0,4,1],</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A7," ","_")  &amp; "_pct' : [" &amp; ROUND(((F7/B7)*-1),2) &amp; "," &amp; ROUND(((E7/B7)*-1),2) &amp; "," &amp; ROUND(((D7/B7)*-1),2)  &amp; "," &amp; ROUND((G7/B7),2) &amp; "," &amp; ROUND((H7/B7),2) &amp; "],"</f>
+        <v>'expert_pct' : [-0.33,-0.11,0,0.44,0.11],</v>
+      </c>
+      <c r="K7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'expert' : [-3,-1,0,4,1],</v>
-      </c>
-      <c r="J7" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L7" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'expert_pct' : [-0.33,-0.11,0,0.44,0.11],</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>318</v>
       </c>
@@ -7565,15 +7827,27 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A8," ","_") &amp; "' : [" &amp; (F8*-1) &amp; "," &amp; (E8*-1) &amp; "," &amp;(D8*-1)&amp; "," &amp; G8 &amp; "," &amp; H8 &amp; "],"</f>
+        <v>'senior' : [0,-4,-3,8,1],</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A8," ","_")  &amp; "_pct' : [" &amp; ROUND(((F8/B8)*-1),2) &amp; "," &amp; ROUND(((E8/B8)*-1),2) &amp; "," &amp; ROUND(((D8/B8)*-1),2)  &amp; "," &amp; ROUND((G8/B8),2) &amp; "," &amp; ROUND((H8/B8),2) &amp; "],"</f>
+        <v>'senior_pct' : [0,-0.25,-0.19,0.5,0.06],</v>
+      </c>
+      <c r="K8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'senior' : [0,-4,-3,8,1],</v>
-      </c>
-      <c r="J8" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
+      </c>
+      <c r="L8" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'senior_pct' : [0,-0.25,-0.19,0.5,0.06],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice','senior'</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>319</v>
       </c>
@@ -7600,37 +7874,61 @@
         <v>0</v>
       </c>
       <c r="I9" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A9," ","_") &amp; "' : [" &amp; (F9*-1) &amp; "," &amp; (E9*-1) &amp; "," &amp;(D9*-1)&amp; "," &amp; G9 &amp; "," &amp; H9 &amp; "],"</f>
+        <v>'novice' : [-1,-2,0,2,0],</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A9," ","_")  &amp; "_pct' : [" &amp; ROUND(((F9/B9)*-1),2) &amp; "," &amp; ROUND(((E9/B9)*-1),2) &amp; "," &amp; ROUND(((D9/B9)*-1),2)  &amp; "," &amp; ROUND((G9/B9),2) &amp; "," &amp; ROUND((H9/B9),2) &amp; "],"</f>
+        <v>'novice_pct' : [-0.2,-0.4,0,0.4,0],</v>
+      </c>
+      <c r="K9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'novice' : [-1,-2,0,2,0],</v>
-      </c>
-      <c r="J9" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
+      </c>
+      <c r="L9" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'novice_pct' : [-0.2,-0.4,0,0.4,0],</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current','novice'</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D10" s="7" t="b">
         <f>SUM(D7:D9)=D2</f>
         <v>1</v>
       </c>
       <c r="E10" s="7" t="b">
-        <f t="shared" ref="E10:H10" si="4">SUM(E7:E9)=E2</f>
+        <f t="shared" ref="E10:H10" si="6">SUM(E7:E9)=E2</f>
         <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H10" s="7" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first','past','current'</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
@@ -7657,15 +7955,27 @@
         <v>0</v>
       </c>
       <c r="I11" s="7" t="str">
+        <f t="shared" ref="I11" si="7">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <v>'current' : [-2,-2,0,8,0],</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A11," ","_")  &amp; "_pct' : [" &amp; ROUND(((F11/B11)*-1),2) &amp; "," &amp; ROUND(((E11/B11)*-1),2) &amp; "," &amp; ROUND(((D11/B11)*-1),2)  &amp; "," &amp; ROUND((G11/B11),2) &amp; "," &amp; ROUND((H11/B11),2) &amp; "],"</f>
+        <v>'current_pct' : [-0.17,-0.17,0,0.67,0],</v>
+      </c>
+      <c r="K11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'current' : [-2,-2,0,8,0],</v>
-      </c>
-      <c r="J11" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'current_pct' : [-0.17,-0.17,0,0.67,0],</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past','current'</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -7692,39 +8002,63 @@
         <v>2</v>
       </c>
       <c r="I12" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A12," ","_") &amp; "' : [" &amp; (F12*-1) &amp; "," &amp; (E12*-1) &amp; "," &amp;(D12*-1)&amp; "," &amp; G12 &amp; "," &amp; H12 &amp; "],"</f>
+        <v>'past' : [-2,-5,-3,6,2],</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A12," ","_")  &amp; "_pct' : [" &amp; ROUND(((F12/B12)*-1),2) &amp; "," &amp; ROUND(((E12/B12)*-1),2) &amp; "," &amp; ROUND(((D12/B12)*-1),2)  &amp; "," &amp; ROUND((G12/B12),2) &amp; "," &amp; ROUND((H12/B12),2) &amp; "],"</f>
+        <v>'past_pct' : [-0.11,-0.28,-0.17,0.33,0.11],</v>
+      </c>
+      <c r="K12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'past' : [-2,-5,-3,6,2],</v>
-      </c>
-      <c r="J12" s="7" t="str">
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx],df.past_pct[xx]</v>
+      </c>
+      <c r="L12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'past_pct' : [-0.11,-0.28,-0.17,0.33,0.11],</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['circuit first','tt first','past'</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx],df.past[xx]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D13" s="7" t="b">
         <f>SUM(D11:D12)=D2</f>
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="5">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="8">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx]</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first'</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.circuit_first[xx],df.tt_first[xx]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B14" s="7">
         <v>14</v>
@@ -7749,17 +8083,29 @@
         <v>1</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14:I15" si="6">"'"&amp;A14 &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
-        <v>'TT First' : [-3,-3,-1,6,1],</v>
+        <f t="shared" ref="I14" si="9">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <v>'tt_first' : [-3,-3,-1,6,1],</v>
       </c>
       <c r="J14" s="7" t="str">
-        <f t="shared" ref="J14:J15" si="7">"'" &amp; A14 &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
-        <v>'TT First_pct' : [-0.21,-0.21,-0.07,0.43,0.07],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A14," ","_")  &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
+        <v>'tt_first_pct' : [-0.21,-0.21,-0.07,0.43,0.07],</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f>IF(ISBLANK(A14),K15,K15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.circuit_first_pct[xx],df.tt_first_pct[xx]</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['circuit first','tt first'</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f>IF(ISBLANK(A14),M15,M15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"[xx]")</f>
+        <v>[df.circuit_first[xx],df.tt_first[xx]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B15" s="7">
         <v>16</v>
@@ -7784,38 +8130,51 @@
         <v>1</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>'Circuit First' : [-1,-4,-2,8,1],</v>
+        <f>"'"&amp;SUBSTITUTE(A15," ","_") &amp; "' : [" &amp; (F15*-1) &amp; "," &amp; (E15*-1) &amp; "," &amp;(D15*-1)&amp; "," &amp; G15 &amp; "," &amp; H15 &amp; "],"</f>
+        <v>'circuit_first' : [-1,-4,-2,8,1],</v>
       </c>
       <c r="J15" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>'Circuit First_pct' : [-0.06,-0.25,-0.13,0.5,0.06],</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A15," ","_")  &amp; "_pct' : [" &amp; ROUND(((F15/B15)*-1),2) &amp; "," &amp; ROUND(((E15/B15)*-1),2) &amp; "," &amp; ROUND(((D15/B15)*-1),2)  &amp; "," &amp; ROUND((G15/B15),2) &amp; "," &amp; ROUND((H15/B15),2) &amp; "],"</f>
+        <v>'circuit_first_pct' : [-0.06,-0.25,-0.13,0.5,0.06],</v>
+      </c>
+      <c r="K15" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A15," ","_") &amp;"_pct[xx]"</f>
+        <v>[df.circuit_first_pct[xx]</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f>"['"&amp; A15&amp;"'"</f>
+        <v>['circuit first'</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A15," ","_") &amp;"[xx]"</f>
+        <v>[df.circuit_first[xx]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D16" s="7" t="b">
         <f>SUM(D14:D15)=D$2</f>
         <v>1</v>
       </c>
       <c r="E16" s="7" t="b">
-        <f t="shared" ref="E16:H16" si="8">SUM(E14:E15)=E$2</f>
+        <f t="shared" ref="E16:H16" si="10">SUM(E14:E15)=E$2</f>
         <v>1</v>
       </c>
       <c r="F16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13024,7 +13383,7 @@
         <v>2</v>
       </c>
       <c r="AF16" s="7">
-        <f>AC16</f>
+        <f t="shared" ref="AF16:AF21" si="5">AC16</f>
         <v>4</v>
       </c>
       <c r="AG16" s="7">
@@ -13150,7 +13509,7 @@
         <v>4</v>
       </c>
       <c r="AF17" s="7">
-        <f>AC17</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AG17" s="7">
@@ -13279,7 +13638,7 @@
         <v>2</v>
       </c>
       <c r="AF18" s="7">
-        <f>AC18</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AG18" s="7">
@@ -13390,7 +13749,7 @@
         <v>5</v>
       </c>
       <c r="AF19" s="7">
-        <f>AC19</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AG19" s="7">
@@ -13513,7 +13872,7 @@
         <v>4</v>
       </c>
       <c r="AF20" s="7">
-        <f>AC20</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AG20" s="7">
@@ -13630,7 +13989,7 @@
         <v>5</v>
       </c>
       <c r="AF21" s="7">
-        <f>AC21</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AG21" s="7">
@@ -13826,7 +14185,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="7">
-        <f t="shared" ref="T24:T29" si="5">W24</f>
+        <f t="shared" ref="T24:T29" si="6">W24</f>
         <v>4</v>
       </c>
       <c r="U24" s="4" t="s">
@@ -13839,7 +14198,7 @@
         <v>4</v>
       </c>
       <c r="X24" s="7">
-        <f t="shared" ref="X24:X29" si="6">S24</f>
+        <f t="shared" ref="X24:X29" si="7">S24</f>
         <v>0</v>
       </c>
       <c r="Y24" s="7" t="s">
@@ -13858,14 +14217,14 @@
         <v>5</v>
       </c>
       <c r="AD24" s="7">
-        <f t="shared" ref="AD24:AD29" si="7">AE24</f>
+        <f t="shared" ref="AD24:AD29" si="8">AE24</f>
         <v>4</v>
       </c>
       <c r="AE24" s="7">
         <v>4</v>
       </c>
       <c r="AF24" s="7">
-        <f>AC24</f>
+        <f t="shared" ref="AF24:AF29" si="9">AC24</f>
         <v>5</v>
       </c>
       <c r="AG24" s="7">
@@ -13943,7 +14302,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="U25" s="4" t="s">
@@ -13956,7 +14315,7 @@
         <v>3</v>
       </c>
       <c r="X25" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y25" s="7" t="s">
@@ -13975,14 +14334,14 @@
         <v>2</v>
       </c>
       <c r="AD25" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AE25" s="7">
         <v>2</v>
       </c>
       <c r="AF25" s="7">
-        <f>AC25</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AG25" s="7">
@@ -14060,7 +14419,7 @@
         <v>0</v>
       </c>
       <c r="T26" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="U26" s="4" t="s">
@@ -14073,7 +14432,7 @@
         <v>5</v>
       </c>
       <c r="X26" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y26" s="7" t="s">
@@ -14092,14 +14451,14 @@
         <v>4</v>
       </c>
       <c r="AD26" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE26" s="7">
         <v>4</v>
       </c>
       <c r="AF26" s="7">
-        <f>AC26</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG26" s="7">
@@ -14183,7 +14542,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U27" s="4" t="s">
@@ -14196,7 +14555,7 @@
         <v>4</v>
       </c>
       <c r="X27" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y27" s="7" t="s">
@@ -14215,14 +14574,14 @@
         <v>1</v>
       </c>
       <c r="AD27" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AE27" s="7">
         <v>1</v>
       </c>
       <c r="AF27" s="7">
-        <f>AC27</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG27" s="7">
@@ -14306,7 +14665,7 @@
         <v>5</v>
       </c>
       <c r="T28" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="U28" s="4" t="s">
@@ -14319,7 +14678,7 @@
         <v>5</v>
       </c>
       <c r="X28" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="Y28" s="7" t="s">
@@ -14338,14 +14697,14 @@
         <v>3</v>
       </c>
       <c r="AD28" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AE28" s="7">
         <v>4</v>
       </c>
       <c r="AF28" s="7">
-        <f>AC28</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AG28" s="7">
@@ -14423,7 +14782,7 @@
         <v>0</v>
       </c>
       <c r="T29" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="U29" s="4" t="s">
@@ -14436,7 +14795,7 @@
         <v>3</v>
       </c>
       <c r="X29" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y29" s="7" t="s">
@@ -14455,14 +14814,14 @@
         <v>4</v>
       </c>
       <c r="AD29" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AE29" s="7">
         <v>5</v>
       </c>
       <c r="AF29" s="7">
-        <f>AC29</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG29" s="7">
@@ -15021,7 +15380,7 @@
         <v>2</v>
       </c>
       <c r="AF35" s="7">
-        <f t="shared" ref="AF35:AF36" si="8">AE35</f>
+        <f t="shared" ref="AF35:AF36" si="10">AE35</f>
         <v>2</v>
       </c>
       <c r="AG35" s="7">
@@ -15141,7 +15500,7 @@
         <v>4</v>
       </c>
       <c r="AF36" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="AG36" s="7">
@@ -15575,7 +15934,7 @@
         <v>3</v>
       </c>
       <c r="AF41" s="7">
-        <f t="shared" ref="AF41:AF44" si="9">AE41</f>
+        <f t="shared" ref="AF41:AF44" si="11">AE41</f>
         <v>3</v>
       </c>
       <c r="AG41" s="7">
@@ -15707,7 +16066,7 @@
         <v>2</v>
       </c>
       <c r="AF42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AG42" s="7">
@@ -15827,7 +16186,7 @@
         <v>3</v>
       </c>
       <c r="AF43" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AG43" s="7">
@@ -15950,7 +16309,7 @@
         <v>2</v>
       </c>
       <c r="AF44" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AG44" s="7">
@@ -16217,11 +16576,11 @@
         <v>3</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I3:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [-1,0,0,6,3],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J3:J12" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f t="shared" ref="J4:J12" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [-0.1,0,0,0.6,0.3],</v>
       </c>
     </row>
@@ -16509,10 +16868,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C22359-5314-43E8-AF1A-50A8F1058A66}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD19"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16522,7 +16881,7 @@
     <col min="10" max="10" width="35.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>315</v>
@@ -16547,9 +16906,9 @@
       </c>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>311</v>
       </c>
@@ -16576,16 +16935,27 @@
         <v>7</v>
       </c>
       <c r="I2" s="7" t="str">
-        <f>"'"&amp;A2 &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A2," ","_") &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
         <v>'total' : [-10,-5,-1,7,7],</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>"'" &amp; A2 &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A2," ","_")  &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
         <v>'total_pct' : [-0.33,-0.17,-0.03,0.23,0.23],</v>
       </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" s="7" t="str">
+        <f>IF(ISBLANK(A2),K3,K3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"_pct[xx]]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx],df.total_pct[xx]]</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>IF(ISBLANK(A2),L3,L3&amp;",'"&amp;A2&amp;"']")</f>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic','total']</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(ISBLANK(A2),M3,M3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"[xx]]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx],df.total[xx]]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -16596,9 +16966,20 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="str">
+        <f>IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f>IF(ISBLANK(A3),L4,L4&amp;",'"&amp; A3 &amp;"'")</f>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f>IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>312</v>
       </c>
@@ -16625,16 +17006,27 @@
         <v>2</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A4," ","_") &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [-4,-3,0,1,2],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J4:J13" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A4," ","_")  &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [-0.4,-0.3,0,0.1,0.2],</v>
       </c>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" s="7" t="str">
+        <f>IF(ISBLANK(A4),K5,K5&amp;",df."&amp; SUBSTITUTE(A4," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" ref="L4:L20" si="1">IF(ISBLANK(A4),L5,L5&amp;",'"&amp; A4 &amp;"'")</f>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f>IF(ISBLANK(A4),M5,M5&amp;",df."&amp; SUBSTITUTE(A4," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>313</v>
       </c>
@@ -16661,16 +17053,27 @@
         <v>5</v>
       </c>
       <c r="I5" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A5," ","_") &amp; "' : [" &amp; (F5*-1) &amp; "," &amp; (E5*-1) &amp; "," &amp;(D5*-1)&amp; "," &amp; G5 &amp; "," &amp; H5 &amp; "],"</f>
+        <v>'practicioner' : [-6,-2,-1,6,5],</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A5," ","_")  &amp; "_pct' : [" &amp; ROUND(((F5/B5)*-1),2) &amp; "," &amp; ROUND(((E5/B5)*-1),2) &amp; "," &amp; ROUND(((D5/B5)*-1),2)  &amp; "," &amp; ROUND((G5/B5),2) &amp; "," &amp; ROUND((H5/B5),2) &amp; "],"</f>
+        <v>'practicioner_pct' : [-0.3,-0.1,-0.05,0.3,0.25],</v>
+      </c>
+      <c r="K5" s="7" t="str">
+        <f>IF(ISBLANK(A5),K6,K6&amp;",df."&amp; SUBSTITUTE(A5," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'practicioner' : [-6,-2,-1,6,5],</v>
-      </c>
-      <c r="J5" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>'practicioner_pct' : [-0.3,-0.1,-0.05,0.3,0.25],</v>
-      </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner'</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f>IF(ISBLANK(A5),M6,M6&amp;",df."&amp; SUBSTITUTE(A5," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -16679,26 +17082,37 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="3">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="2">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K6" s="7" t="str">
+        <f>IF(ISBLANK(A6),K7,K7&amp;",df."&amp; SUBSTITUTE(A6," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f>IF(ISBLANK(A6),M7,M7&amp;",df."&amp; SUBSTITUTE(A6," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>317</v>
       </c>
@@ -16725,16 +17139,27 @@
         <v>2</v>
       </c>
       <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7" si="3">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <v>'expert' : [-3,-1,-1,2,2],</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A7," ","_")  &amp; "_pct' : [" &amp; ROUND(((F7/B7)*-1),2) &amp; "," &amp; ROUND(((E7/B7)*-1),2) &amp; "," &amp; ROUND(((D7/B7)*-1),2)  &amp; "," &amp; ROUND((G7/B7),2) &amp; "," &amp; ROUND((H7/B7),2) &amp; "],"</f>
+        <v>'expert_pct' : [-0.33,-0.11,-0.11,0.22,0.22],</v>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f>IF(ISBLANK(A7),K8,K8&amp;",df."&amp; SUBSTITUTE(A7," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'expert' : [-3,-1,-1,2,2],</v>
-      </c>
-      <c r="J7" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>'expert_pct' : [-0.33,-0.11,-0.11,0.22,0.22],</v>
-      </c>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f>IF(ISBLANK(A7),M8,M8&amp;",df."&amp; SUBSTITUTE(A7," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>318</v>
       </c>
@@ -16761,16 +17186,27 @@
         <v>4</v>
       </c>
       <c r="I8" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A8," ","_") &amp; "' : [" &amp; (F8*-1) &amp; "," &amp; (E8*-1) &amp; "," &amp;(D8*-1)&amp; "," &amp; G8 &amp; "," &amp; H8 &amp; "],"</f>
+        <v>'senior' : [-5,-2,0,5,4],</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A8," ","_")  &amp; "_pct' : [" &amp; ROUND(((F8/B8)*-1),2) &amp; "," &amp; ROUND(((E8/B8)*-1),2) &amp; "," &amp; ROUND(((D8/B8)*-1),2)  &amp; "," &amp; ROUND((G8/B8),2) &amp; "," &amp; ROUND((H8/B8),2) &amp; "],"</f>
+        <v>'senior_pct' : [-0.31,-0.13,0,0.31,0.25],</v>
+      </c>
+      <c r="K8" s="7" t="str">
+        <f>IF(ISBLANK(A8),K9,K9&amp;",df."&amp; SUBSTITUTE(A8," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
+      </c>
+      <c r="L8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'senior' : [-5,-2,0,5,4],</v>
-      </c>
-      <c r="J8" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>'senior_pct' : [-0.31,-0.13,0,0.31,0.25],</v>
-      </c>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior'</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f>IF(ISBLANK(A8),M9,M9&amp;",df."&amp; SUBSTITUTE(A8," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>319</v>
       </c>
@@ -16797,16 +17233,27 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A9," ","_") &amp; "' : [" &amp; (F9*-1) &amp; "," &amp; (E9*-1) &amp; "," &amp;(D9*-1)&amp; "," &amp; G9 &amp; "," &amp; H9 &amp; "],"</f>
+        <v>'novice' : [-2,-2,0,0,1],</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A9," ","_")  &amp; "_pct' : [" &amp; ROUND(((F9/B9)*-1),2) &amp; "," &amp; ROUND(((E9/B9)*-1),2) &amp; "," &amp; ROUND(((D9/B9)*-1),2)  &amp; "," &amp; ROUND((G9/B9),2) &amp; "," &amp; ROUND((H9/B9),2) &amp; "],"</f>
+        <v>'novice_pct' : [-0.4,-0.4,0,0,0.2],</v>
+      </c>
+      <c r="K9" s="7" t="str">
+        <f>IF(ISBLANK(A9),K10,K10&amp;",df."&amp; SUBSTITUTE(A9," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
+      </c>
+      <c r="L9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'novice' : [-2,-2,0,0,1],</v>
-      </c>
-      <c r="J9" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>'novice_pct' : [-0.4,-0.4,0,0,0.2],</v>
-      </c>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice'</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f>IF(ISBLANK(A9),M10,M10&amp;",df."&amp; SUBSTITUTE(A9," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -16832,9 +17279,20 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" s="7" t="str">
+        <f>IF(ISBLANK(A10),K11,K11&amp;",df."&amp; SUBSTITUTE(A10," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f>IF(ISBLANK(A10),M11,M11&amp;",df."&amp; SUBSTITUTE(A10," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
@@ -16861,16 +17319,27 @@
         <v>2</v>
       </c>
       <c r="I11" s="7" t="str">
+        <f t="shared" ref="I11" si="5">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <v>'current' : [-5,-2,-1,2,2],</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A11," ","_")  &amp; "_pct' : [" &amp; ROUND(((F11/B11)*-1),2) &amp; "," &amp; ROUND(((E11/B11)*-1),2) &amp; "," &amp; ROUND(((D11/B11)*-1),2)  &amp; "," &amp; ROUND((G11/B11),2) &amp; "," &amp; ROUND((H11/B11),2) &amp; "],"</f>
+        <v>'current_pct' : [-0.42,-0.17,-0.08,0.17,0.17],</v>
+      </c>
+      <c r="K11" s="7" t="str">
+        <f>IF(ISBLANK(A11),K12,K12&amp;",df."&amp; SUBSTITUTE(A11," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'current' : [-5,-2,-1,2,2],</v>
-      </c>
-      <c r="J11" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>'current_pct' : [-0.42,-0.17,-0.08,0.17,0.17],</v>
-      </c>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f>IF(ISBLANK(A11),M12,M12&amp;",df."&amp; SUBSTITUTE(A11," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -16897,16 +17366,27 @@
         <v>5</v>
       </c>
       <c r="I12" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A12," ","_") &amp; "' : [" &amp; (F12*-1) &amp; "," &amp; (E12*-1) &amp; "," &amp;(D12*-1)&amp; "," &amp; G12 &amp; "," &amp; H12 &amp; "],"</f>
+        <v>'past' : [-5,-3,0,5,5],</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A12," ","_")  &amp; "_pct' : [" &amp; ROUND(((F12/B12)*-1),2) &amp; "," &amp; ROUND(((E12/B12)*-1),2) &amp; "," &amp; ROUND(((D12/B12)*-1),2)  &amp; "," &amp; ROUND((G12/B12),2) &amp; "," &amp; ROUND((H12/B12),2) &amp; "],"</f>
+        <v>'past_pct' : [-0.28,-0.17,0,0.28,0.28],</v>
+      </c>
+      <c r="K12" s="7" t="str">
+        <f>IF(ISBLANK(A12),K13,K13&amp;",df."&amp; SUBSTITUTE(A12," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx]</v>
+      </c>
+      <c r="L12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'past' : [-5,-3,0,5,5],</v>
-      </c>
-      <c r="J12" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>'past_pct' : [-0.28,-0.17,0,0.28,0.28],</v>
-      </c>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past'</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f>IF(ISBLANK(A12),M13,M13&amp;",df."&amp; SUBSTITUTE(A12," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -16915,26 +17395,37 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="5">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="6">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K13" s="7" t="str">
+        <f>IF(ISBLANK(A13),K14,K14&amp;",df."&amp; SUBSTITUTE(A13," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table'</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f>IF(ISBLANK(A13),M14,M14&amp;",df."&amp; SUBSTITUTE(A13," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>326</v>
       </c>
@@ -16961,16 +17452,27 @@
         <v>1</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14:I15" si="6">"'"&amp;A14 &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
-        <v>'decision table' : [-4,-5,0,2,1],</v>
+        <f t="shared" ref="I14" si="7">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <v>'decision_table' : [-4,-5,0,2,1],</v>
       </c>
       <c r="J14" s="7" t="str">
-        <f t="shared" ref="J14:J15" si="7">"'" &amp; A14 &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
-        <v>'decision table_pct' : [-0.33,-0.42,0,0.17,0.08],</v>
-      </c>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A14," ","_")  &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
+        <v>'decision_table_pct' : [-0.33,-0.42,0,0.17,0.08],</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f>IF(ISBLANK(A14),K15,K15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table'</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f>IF(ISBLANK(A14),M15,M15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>327</v>
       </c>
@@ -16997,15 +17499,27 @@
         <v>6</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f>"'"&amp;SUBSTITUTE(A15," ","_") &amp; "' : [" &amp; (F15*-1) &amp; "," &amp; (E15*-1) &amp; "," &amp;(D15*-1)&amp; "," &amp; G15 &amp; "," &amp; H15 &amp; "],"</f>
         <v>'spreadsheet' : [-6,0,-1,5,6],</v>
       </c>
       <c r="J15" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f>"'" &amp; SUBSTITUTE(A15," ","_")  &amp; "_pct' : [" &amp; ROUND(((F15/B15)*-1),2) &amp; "," &amp; ROUND(((E15/B15)*-1),2) &amp; "," &amp; ROUND(((D15/B15)*-1),2)  &amp; "," &amp; ROUND((G15/B15),2) &amp; "," &amp; ROUND((H15/B15),2) &amp; "],"</f>
         <v>'spreadsheet_pct' : [-0.33,0,-0.06,0.28,0.33],</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K15" s="7" t="str">
+        <f>IF(ISBLANK(A15),K16,K16&amp;",df."&amp; SUBSTITUTE(A15," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx]</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1','spreadsheet'</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f>IF(ISBLANK(A15),M16,M16&amp;",df."&amp; SUBSTITUTE(A15," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D16" t="b">
         <f>SUM(D14:D15)=D$2</f>
         <v>1</v>
@@ -17026,8 +17540,20 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" s="7" t="str">
+        <f>IF(ISBLANK(A16),K17,K17&amp;",df."&amp; SUBSTITUTE(A16," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M16" s="7" t="str">
+        <f>IF(ISBLANK(A16),M17,M17&amp;",df."&amp; SUBSTITUTE(A16," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>328</v>
       </c>
@@ -17054,15 +17580,27 @@
         <v>3</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" ref="I17:I18" si="9">"'"&amp;A17 &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
-        <v>'ruleset 1' : [-6,-3,-1,5,3],</v>
+        <f t="shared" ref="I17" si="9">"'"&amp;SUBSTITUTE(A17," ","_") &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
+        <v>'ruleset_1' : [-6,-3,-1,5,3],</v>
       </c>
       <c r="J17" s="7" t="str">
-        <f t="shared" ref="J17:J18" si="10">"'" &amp; A17 &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
-        <v>'ruleset 1_pct' : [-0.33,-0.17,-0.06,0.28,0.17],</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A17," ","_")  &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
+        <v>'ruleset_1_pct' : [-0.33,-0.17,-0.06,0.28,0.17],</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f>IF(ISBLANK(A17),K18,K18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f>IF(ISBLANK(A17),M18,M18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>329</v>
       </c>
@@ -17089,38 +17627,62 @@
         <v>4</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>'ruleset 2' : [-4,-2,0,2,4],</v>
+        <f>"'"&amp;SUBSTITUTE(A18," ","_") &amp; "' : [" &amp; (F18*-1) &amp; "," &amp; (E18*-1) &amp; "," &amp;(D18*-1)&amp; "," &amp; G18 &amp; "," &amp; H18 &amp; "],"</f>
+        <v>'ruleset_2' : [-4,-2,0,2,4],</v>
       </c>
       <c r="J18" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>'ruleset 2_pct' : [-0.33,-0.17,0,0.17,0.33],</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A18," ","_")  &amp; "_pct' : [" &amp; ROUND(((F18/B18)*-1),2) &amp; "," &amp; ROUND(((E18/B18)*-1),2) &amp; "," &amp; ROUND(((D18/B18)*-1),2)  &amp; "," &amp; ROUND((G18/B18),2) &amp; "," &amp; ROUND((H18/B18),2) &amp; "],"</f>
+        <v>'ruleset_2_pct' : [-0.33,-0.17,0,0.17,0.33],</v>
+      </c>
+      <c r="K18" s="7" t="str">
+        <f>IF(ISBLANK(A18),K19,K19&amp;",df."&amp; SUBSTITUTE(A18," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx]</v>
+      </c>
+      <c r="L18" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection','ruleset 2'</v>
+      </c>
+      <c r="M18" s="7" t="str">
+        <f>IF(ISBLANK(A18),M19,M19&amp;",df."&amp; SUBSTITUTE(A18," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="b">
         <f>SUM(D17:D18)=D$2</f>
         <v>1</v>
       </c>
       <c r="E19" s="7" t="b">
-        <f t="shared" ref="E19" si="11">SUM(E17:E18)=E$2</f>
+        <f t="shared" ref="E19" si="10">SUM(E17:E18)=E$2</f>
         <v>1</v>
       </c>
       <c r="F19" s="7" t="b">
-        <f t="shared" ref="F19" si="12">SUM(F17:F18)=F$2</f>
+        <f t="shared" ref="F19" si="11">SUM(F17:F18)=F$2</f>
         <v>1</v>
       </c>
       <c r="G19" s="7" t="b">
-        <f t="shared" ref="G19" si="13">SUM(G17:G18)=G$2</f>
+        <f t="shared" ref="G19" si="12">SUM(G17:G18)=G$2</f>
         <v>1</v>
       </c>
       <c r="H19" s="7" t="b">
-        <f t="shared" ref="H19" si="14">SUM(H17:H18)=H$2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" ref="H19" si="13">SUM(H17:H18)=H$2</f>
+        <v>1</v>
+      </c>
+      <c r="K19" s="7" t="str">
+        <f>IF(ISBLANK(A19),K20,K20&amp;",df."&amp; SUBSTITUTE(A19," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx]</v>
+      </c>
+      <c r="L19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection'</v>
+      </c>
+      <c r="M19" s="7" t="str">
+        <f>IF(ISBLANK(A19),M20,M20&amp;",df."&amp; SUBSTITUTE(A19," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>297</v>
       </c>
@@ -17147,15 +17709,27 @@
         <v>3</v>
       </c>
       <c r="I20" s="7" t="str">
-        <f t="shared" ref="I20:I21" si="15">"'"&amp;A20 &amp; "' : [" &amp; (F20*-1) &amp; "," &amp; (E20*-1) &amp; "," &amp;(D20*-1)&amp; "," &amp; G20 &amp; "," &amp; H20 &amp; "],"</f>
+        <f t="shared" ref="I20" si="14">"'"&amp;SUBSTITUTE(A20," ","_") &amp; "' : [" &amp; (F20*-1) &amp; "," &amp; (E20*-1) &amp; "," &amp;(D20*-1)&amp; "," &amp; G20 &amp; "," &amp; H20 &amp; "],"</f>
         <v>'projection' : [-6,-3,0,2,3],</v>
       </c>
       <c r="J20" s="7" t="str">
-        <f t="shared" ref="J20:J21" si="16">"'" &amp; A20 &amp; "_pct' : [" &amp; ROUND(((F20/B20)*-1),2) &amp; "," &amp; ROUND(((E20/B20)*-1),2) &amp; "," &amp; ROUND(((D20/B20)*-1),2)  &amp; "," &amp; ROUND((G20/B20),2) &amp; "," &amp; ROUND((H20/B20),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A20," ","_")  &amp; "_pct' : [" &amp; ROUND(((F20/B20)*-1),2) &amp; "," &amp; ROUND(((E20/B20)*-1),2) &amp; "," &amp; ROUND(((D20/B20)*-1),2)  &amp; "," &amp; ROUND((G20/B20),2) &amp; "," &amp; ROUND((H20/B20),2) &amp; "],"</f>
         <v>'projection_pct' : [-0.43,-0.21,0,0.14,0.21],</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" s="7" t="str">
+        <f>IF(ISBLANK(A20),K21,K21&amp;",df."&amp; SUBSTITUTE(A20," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx]</v>
+      </c>
+      <c r="L20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>['text','projection'</v>
+      </c>
+      <c r="M20" t="str">
+        <f>IF(ISBLANK(A20),M21,M21&amp;",df."&amp; SUBSTITUTE(A20," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>334</v>
       </c>
@@ -17182,33 +17756,45 @@
         <v>4</v>
       </c>
       <c r="I21" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f>"'"&amp;SUBSTITUTE(A21," ","_") &amp; "' : [" &amp; (F21*-1) &amp; "," &amp; (E21*-1) &amp; "," &amp;(D21*-1)&amp; "," &amp; G21 &amp; "," &amp; H21 &amp; "],"</f>
         <v>'text' : [-4,-2,-1,5,4],</v>
       </c>
       <c r="J21" s="7" t="str">
-        <f t="shared" si="16"/>
+        <f>"'" &amp; SUBSTITUTE(A21," ","_")  &amp; "_pct' : [" &amp; ROUND(((F21/B21)*-1),2) &amp; "," &amp; ROUND(((E21/B21)*-1),2) &amp; "," &amp; ROUND(((D21/B21)*-1),2)  &amp; "," &amp; ROUND((G21/B21),2) &amp; "," &amp; ROUND((H21/B21),2) &amp; "],"</f>
         <v>'text_pct' : [-0.25,-0.13,-0.06,0.31,0.25],</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A21," ","_") &amp;"_pct[xx]"</f>
+        <v>[df.text_pct[xx]</v>
+      </c>
+      <c r="L21" t="str">
+        <f>"['"&amp; A21 &amp;"'"</f>
+        <v>['text'</v>
+      </c>
+      <c r="M21" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A21," ","_") &amp;"[xx]"</f>
+        <v>[df.text[xx]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D22" s="7" t="b">
         <f>SUM(D20:D21)=D$2</f>
         <v>1</v>
       </c>
       <c r="E22" s="7" t="b">
-        <f t="shared" ref="E22" si="17">SUM(E20:E21)=E$2</f>
+        <f t="shared" ref="E22" si="15">SUM(E20:E21)=E$2</f>
         <v>1</v>
       </c>
       <c r="F22" s="7" t="b">
-        <f t="shared" ref="F22" si="18">SUM(F20:F21)=F$2</f>
+        <f t="shared" ref="F22" si="16">SUM(F20:F21)=F$2</f>
         <v>1</v>
       </c>
       <c r="G22" s="7" t="b">
-        <f t="shared" ref="G22" si="19">SUM(G20:G21)=G$2</f>
+        <f t="shared" ref="G22" si="17">SUM(G20:G21)=G$2</f>
         <v>1</v>
       </c>
       <c r="H22" s="7" t="b">
-        <f t="shared" ref="H22" si="20">SUM(H20:H21)=H$2</f>
+        <f t="shared" ref="H22" si="18">SUM(H20:H21)=H$2</f>
         <v>1</v>
       </c>
     </row>
@@ -17219,15 +17805,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D893DAA-EFB1-4118-8F7B-F1D73DB3BFF6}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K2" sqref="K2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>315</v>
@@ -17253,7 +17839,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>311</v>
       </c>
@@ -17280,15 +17866,27 @@
         <v>5</v>
       </c>
       <c r="I2" s="7" t="str">
-        <f>"'"&amp;A2 &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A2," ","_") &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
         <v>'total' : [-5,-1,-1,6,5],</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>"'" &amp; A2 &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A2," ","_")  &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
         <v>'total_pct' : [-0.28,-0.06,-0.06,0.33,0.28],</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="7" t="str">
+        <f>IF(ISBLANK(A2),K3,K3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"_pct[xx]]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx],df.total_pct[xx]]</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>IF(ISBLANK(A2),L3,L3&amp;",'"&amp; A2 &amp;"']")</f>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior','expert','practicioner','academic','total']</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>IF(ISBLANK(A2),M3,M3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"[xx]]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx],df.total[xx]]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -17299,8 +17897,20 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K16" si="1">IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f>IF(ISBLANK(A3),L4,L4&amp;",'"&amp; A3 &amp;"'")</f>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f t="shared" ref="M3:M16" si="2">IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>312</v>
       </c>
@@ -17327,15 +17937,27 @@
         <v>2</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A4," ","_") &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [-3,-1,0,2,2],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J4:J12" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A4," ","_")  &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [-0.38,-0.13,0,0.25,0.25],</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" ref="L4:L17" si="3">IF(ISBLANK(A4),L5,L5&amp;",'"&amp; A4 &amp;"'")</f>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>313</v>
       </c>
@@ -17362,15 +17984,27 @@
         <v>3</v>
       </c>
       <c r="I5" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A5," ","_") &amp; "' : [" &amp; (F5*-1) &amp; "," &amp; (E5*-1) &amp; "," &amp;(D5*-1)&amp; "," &amp; G5 &amp; "," &amp; H5 &amp; "],"</f>
+        <v>'practicioner' : [-2,0,-1,4,3],</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A5," ","_")  &amp; "_pct' : [" &amp; ROUND(((F5/B5)*-1),2) &amp; "," &amp; ROUND(((E5/B5)*-1),2) &amp; "," &amp; ROUND(((D5/B5)*-1),2)  &amp; "," &amp; ROUND((G5/B5),2) &amp; "," &amp; ROUND((H5/B5),2) &amp; "],"</f>
+        <v>'practicioner_pct' : [-0.2,0,-0.1,0.4,0.3],</v>
+      </c>
+      <c r="K5" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'practicioner' : [-2,0,-1,4,3],</v>
-      </c>
-      <c r="J5" s="7" t="str">
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
+      </c>
+      <c r="L5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior','expert','practicioner'</v>
+      </c>
+      <c r="M5" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'practicioner_pct' : [-0.2,0,-0.1,0.4,0.3],</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -17379,25 +18013,37 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="3">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="4">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>317</v>
       </c>
@@ -17424,15 +18070,27 @@
         <v>3</v>
       </c>
       <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7" si="5">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <v>'expert' : [-1,0,-1,1,3],</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A7," ","_")  &amp; "_pct' : [" &amp; ROUND(((F7/B7)*-1),2) &amp; "," &amp; ROUND(((E7/B7)*-1),2) &amp; "," &amp; ROUND(((D7/B7)*-1),2)  &amp; "," &amp; ROUND((G7/B7),2) &amp; "," &amp; ROUND((H7/B7),2) &amp; "],"</f>
+        <v>'expert_pct' : [-0.17,0,-0.17,0.17,0.5],</v>
+      </c>
+      <c r="K7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'expert' : [-1,0,-1,1,3],</v>
-      </c>
-      <c r="J7" s="7" t="str">
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M7" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'expert_pct' : [-0.17,0,-0.17,0.17,0.5],</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>318</v>
       </c>
@@ -17459,15 +18117,27 @@
         <v>2</v>
       </c>
       <c r="I8" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A8," ","_") &amp; "' : [" &amp; (F8*-1) &amp; "," &amp; (E8*-1) &amp; "," &amp;(D8*-1)&amp; "," &amp; G8 &amp; "," &amp; H8 &amp; "],"</f>
+        <v>'senior' : [-2,-1,0,3,2],</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A8," ","_")  &amp; "_pct' : [" &amp; ROUND(((F8/B8)*-1),2) &amp; "," &amp; ROUND(((E8/B8)*-1),2) &amp; "," &amp; ROUND(((D8/B8)*-1),2)  &amp; "," &amp; ROUND((G8/B8),2) &amp; "," &amp; ROUND((H8/B8),2) &amp; "],"</f>
+        <v>'senior_pct' : [-0.25,-0.13,0,0.38,0.25],</v>
+      </c>
+      <c r="K8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'senior' : [-2,-1,0,3,2],</v>
-      </c>
-      <c r="J8" s="7" t="str">
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
+      </c>
+      <c r="L8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice','senior'</v>
+      </c>
+      <c r="M8" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'senior_pct' : [-0.25,-0.13,0,0.38,0.25],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>319</v>
       </c>
@@ -17494,15 +18164,27 @@
         <v>0</v>
       </c>
       <c r="I9" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A9," ","_") &amp; "' : [" &amp; (F9*-1) &amp; "," &amp; (E9*-1) &amp; "," &amp;(D9*-1)&amp; "," &amp; G9 &amp; "," &amp; H9 &amp; "],"</f>
+        <v>'novice' : [-2,0,0,2,0],</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A9," ","_")  &amp; "_pct' : [" &amp; ROUND(((F9/B9)*-1),2) &amp; "," &amp; ROUND(((E9/B9)*-1),2) &amp; "," &amp; ROUND(((D9/B9)*-1),2)  &amp; "," &amp; ROUND((G9/B9),2) &amp; "," &amp; ROUND((H9/B9),2) &amp; "],"</f>
+        <v>'novice_pct' : [-0.5,0,0,0.5,0],</v>
+      </c>
+      <c r="K9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'novice' : [-2,0,0,2,0],</v>
-      </c>
-      <c r="J9" s="7" t="str">
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
+      </c>
+      <c r="L9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current','novice'</v>
+      </c>
+      <c r="M9" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'novice_pct' : [-0.5,0,0,0.5,0],</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -17511,25 +18193,37 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="b">
-        <f t="shared" ref="E10:H10" si="4">SUM(E7:E9)=E2</f>
+        <f t="shared" ref="E10:H10" si="6">SUM(E7:E9)=E2</f>
         <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current'</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
@@ -17556,15 +18250,27 @@
         <v>2</v>
       </c>
       <c r="I11" s="7" t="str">
+        <f t="shared" ref="I11" si="7">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <v>'current' : [-1,0,-1,1,2],</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A11," ","_")  &amp; "_pct' : [" &amp; ROUND(((F11/B11)*-1),2) &amp; "," &amp; ROUND(((E11/B11)*-1),2) &amp; "," &amp; ROUND(((D11/B11)*-1),2)  &amp; "," &amp; ROUND((G11/B11),2) &amp; "," &amp; ROUND((H11/B11),2) &amp; "],"</f>
+        <v>'current_pct' : [-0.2,0,-0.2,0.2,0.4],</v>
+      </c>
+      <c r="K11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'current' : [-1,0,-1,1,2],</v>
-      </c>
-      <c r="J11" s="7" t="str">
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past','current'</v>
+      </c>
+      <c r="M11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'current_pct' : [-0.2,0,-0.2,0.2,0.4],</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -17591,15 +18297,27 @@
         <v>3</v>
       </c>
       <c r="I12" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A12," ","_") &amp; "' : [" &amp; (F12*-1) &amp; "," &amp; (E12*-1) &amp; "," &amp;(D12*-1)&amp; "," &amp; G12 &amp; "," &amp; H12 &amp; "],"</f>
+        <v>'past' : [-4,-1,0,5,3],</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A12," ","_")  &amp; "_pct' : [" &amp; ROUND(((F12/B12)*-1),2) &amp; "," &amp; ROUND(((E12/B12)*-1),2) &amp; "," &amp; ROUND(((D12/B12)*-1),2)  &amp; "," &amp; ROUND((G12/B12),2) &amp; "," &amp; ROUND((H12/B12),2) &amp; "],"</f>
+        <v>'past_pct' : [-0.31,-0.08,0,0.38,0.23],</v>
+      </c>
+      <c r="K12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'past' : [-4,-1,0,5,3],</v>
-      </c>
-      <c r="J12" s="7" t="str">
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.past_pct[xx]</v>
+      </c>
+      <c r="L12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1','past'</v>
+      </c>
+      <c r="M12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'past_pct' : [-0.31,-0.08,0,0.38,0.23],</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.past[xx]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -17608,25 +18326,37 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="5">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="8">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>328</v>
       </c>
@@ -17653,15 +18383,27 @@
         <v>1</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14:I15" si="6">"'"&amp;A14 &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
-        <v>'ruleset 1' : [-4,-1,0,3,1],</v>
+        <f t="shared" ref="I14" si="9">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <v>'ruleset_1' : [-4,-1,0,3,1],</v>
       </c>
       <c r="J14" s="7" t="str">
-        <f t="shared" ref="J14:J15" si="7">"'" &amp; A14 &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
-        <v>'ruleset 1_pct' : [-0.44,-0.11,0,0.33,0.11],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A14," ","_")  &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
+        <v>'ruleset_1_pct' : [-0.44,-0.11,0,0.33,0.11],</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>329</v>
       </c>
@@ -17688,15 +18430,27 @@
         <v>4</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>'ruleset 2' : [-1,0,-1,3,4],</v>
+        <f>"'"&amp;SUBSTITUTE(A15," ","_") &amp; "' : [" &amp; (F15*-1) &amp; "," &amp; (E15*-1) &amp; "," &amp;(D15*-1)&amp; "," &amp; G15 &amp; "," &amp; H15 &amp; "],"</f>
+        <v>'ruleset_2' : [-1,0,-1,3,4],</v>
       </c>
       <c r="J15" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>'ruleset 2_pct' : [-0.11,0,-0.11,0.33,0.44],</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A15," ","_")  &amp; "_pct' : [" &amp; ROUND(((F15/B15)*-1),2) &amp; "," &amp; ROUND(((E15/B15)*-1),2) &amp; "," &amp; ROUND(((D15/B15)*-1),2)  &amp; "," &amp; ROUND((G15/B15),2) &amp; "," &amp; ROUND((H15/B15),2) &amp; "],"</f>
+        <v>'ruleset_2_pct' : [-0.11,0,-0.11,0.33,0.44],</v>
+      </c>
+      <c r="K15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx]</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection','ruleset 2'</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -17705,25 +18459,37 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="b">
-        <f t="shared" ref="E16:H16" si="8">SUM(E14:E15)=E$2</f>
+        <f t="shared" ref="E16:H16" si="10">SUM(E14:E15)=E$2</f>
         <v>1</v>
       </c>
       <c r="F16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.text_pct[xx],df.projection_pct[xx]</v>
+      </c>
+      <c r="L16" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection'</v>
+      </c>
+      <c r="M16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>[df.text[xx],df.projection[xx]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>297</v>
       </c>
@@ -17750,15 +18516,27 @@
         <v>3</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" ref="I17:I18" si="9">"'"&amp;A17 &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
+        <f t="shared" ref="I17" si="11">"'"&amp;SUBSTITUTE(A17," ","_") &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
         <v>'projection' : [-5,-1,0,5,3],</v>
       </c>
       <c r="J17" s="7" t="str">
-        <f t="shared" ref="J17:J18" si="10">"'" &amp; A17 &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A17," ","_")  &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
         <v>'projection_pct' : [-0.36,-0.07,0,0.36,0.21],</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" s="7" t="str">
+        <f>IF(ISBLANK(A17),K18,K18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.text_pct[xx],df.projection_pct[xx]</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>['text','projection'</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f>IF(ISBLANK(A17),M18,M18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"[xx]")</f>
+        <v>[df.text[xx],df.projection[xx]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>334</v>
       </c>
@@ -17785,15 +18563,27 @@
         <v>2</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="9"/>
+        <f>"'"&amp;SUBSTITUTE(A18," ","_") &amp; "' : [" &amp; (F18*-1) &amp; "," &amp; (E18*-1) &amp; "," &amp;(D18*-1)&amp; "," &amp; G18 &amp; "," &amp; H18 &amp; "],"</f>
         <v>'text' : [0,0,-1,1,2],</v>
       </c>
       <c r="J18" s="7" t="str">
-        <f t="shared" si="10"/>
+        <f>"'" &amp; SUBSTITUTE(A18," ","_")  &amp; "_pct' : [" &amp; ROUND(((F18/B18)*-1),2) &amp; "," &amp; ROUND(((E18/B18)*-1),2) &amp; "," &amp; ROUND(((D18/B18)*-1),2)  &amp; "," &amp; ROUND((G18/B18),2) &amp; "," &amp; ROUND((H18/B18),2) &amp; "],"</f>
         <v>'text_pct' : [0,0,-0.25,0.25,0.5],</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A18," ","_") &amp;"_pct[xx]"</f>
+        <v>[df.text_pct[xx]</v>
+      </c>
+      <c r="L18" s="7" t="str">
+        <f>"['"&amp; A18&amp;"'"</f>
+        <v>['text'</v>
+      </c>
+      <c r="M18" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A18," ","_") &amp;"[xx]"</f>
+        <v>[df.text[xx]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -17802,23 +18592,31 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="b">
-        <f t="shared" ref="E19:H19" si="11">SUM(E17:E18)=E$2</f>
+        <f t="shared" ref="E19:H19" si="12">SUM(E17:E18)=E$2</f>
         <v>1</v>
       </c>
       <c r="F19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17827,10 +18625,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2189D71-B2C2-470B-B11E-70CE459BF187}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J19"/>
+      <selection activeCell="K2" sqref="K2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17843,7 +18641,7 @@
     <col min="10" max="10" width="35.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>315</v>
@@ -17870,7 +18668,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>311</v>
       </c>
@@ -17897,16 +18695,27 @@
         <v>1</v>
       </c>
       <c r="I2" s="7" t="str">
-        <f>"'"&amp;A2 &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A2," ","_") &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
         <v>'total' : [-3,-7,-4,15,1],</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>"'" &amp; A2 &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A2," ","_")  &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
         <v>'total_pct' : [-0.1,-0.23,-0.13,0.5,0.03],</v>
       </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" s="7" t="str">
+        <f>IF(ISBLANK(A2),K3,K3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"_pct[xx]]")</f>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx],df.total_pct[xx]]</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>IF(ISBLANK(A2),L3,L3&amp;",'"&amp; A2 &amp;"']")</f>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic','total']</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>IF(ISBLANK(A2),M3,M3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"[xx]]")</f>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx],df.total[xx]]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -17917,9 +18726,20 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K16" si="1">IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="shared" ref="L3:L16" si="2">IF(ISBLANK(A3),L4,L4&amp;",'"&amp; A3 &amp;"'")</f>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f t="shared" ref="M3:M16" si="3">IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>312</v>
       </c>
@@ -17946,16 +18766,27 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A4," ","_") &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [-2,-2,0,5,1],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J4:J13" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A4," ","_")  &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [-0.2,-0.2,0,0.5,0.1],</v>
       </c>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>313</v>
       </c>
@@ -17982,16 +18813,27 @@
         <v>0</v>
       </c>
       <c r="I5" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A5," ","_") &amp; "' : [" &amp; (F5*-1) &amp; "," &amp; (E5*-1) &amp; "," &amp;(D5*-1)&amp; "," &amp; G5 &amp; "," &amp; H5 &amp; "],"</f>
+        <v>'practicioner' : [-1,-5,-4,10,0],</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A5," ","_")  &amp; "_pct' : [" &amp; ROUND(((F5/B5)*-1),2) &amp; "," &amp; ROUND(((E5/B5)*-1),2) &amp; "," &amp; ROUND(((D5/B5)*-1),2)  &amp; "," &amp; ROUND((G5/B5),2) &amp; "," &amp; ROUND((H5/B5),2) &amp; "],"</f>
+        <v>'practicioner_pct' : [-0.05,-0.25,-0.2,0.5,0],</v>
+      </c>
+      <c r="K5" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'practicioner' : [-1,-5,-4,10,0],</v>
-      </c>
-      <c r="J5" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'practicioner_pct' : [-0.05,-0.25,-0.2,0.5,0],</v>
-      </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner'</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -18000,26 +18842,37 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="3">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="4">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>317</v>
       </c>
@@ -18046,16 +18899,27 @@
         <v>0</v>
       </c>
       <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7" si="5">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <v>'expert' : [0,-3,-2,4,0],</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A7," ","_")  &amp; "_pct' : [" &amp; ROUND(((F7/B7)*-1),2) &amp; "," &amp; ROUND(((E7/B7)*-1),2) &amp; "," &amp; ROUND(((D7/B7)*-1),2)  &amp; "," &amp; ROUND((G7/B7),2) &amp; "," &amp; ROUND((H7/B7),2) &amp; "],"</f>
+        <v>'expert_pct' : [0,-0.33,-0.22,0.44,0],</v>
+      </c>
+      <c r="K7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'expert' : [0,-3,-2,4,0],</v>
-      </c>
-      <c r="J7" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L7" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'expert_pct' : [0,-0.33,-0.22,0.44,0],</v>
-      </c>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>318</v>
       </c>
@@ -18082,16 +18946,27 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A8," ","_") &amp; "' : [" &amp; (F8*-1) &amp; "," &amp; (E8*-1) &amp; "," &amp;(D8*-1)&amp; "," &amp; G8 &amp; "," &amp; H8 &amp; "],"</f>
+        <v>'senior' : [-2,-3,-2,9,0],</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A8," ","_")  &amp; "_pct' : [" &amp; ROUND(((F8/B8)*-1),2) &amp; "," &amp; ROUND(((E8/B8)*-1),2) &amp; "," &amp; ROUND(((D8/B8)*-1),2)  &amp; "," &amp; ROUND((G8/B8),2) &amp; "," &amp; ROUND((H8/B8),2) &amp; "],"</f>
+        <v>'senior_pct' : [-0.13,-0.19,-0.13,0.56,0],</v>
+      </c>
+      <c r="K8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'senior' : [-2,-3,-2,9,0],</v>
-      </c>
-      <c r="J8" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
+      </c>
+      <c r="L8" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'senior_pct' : [-0.13,-0.19,-0.13,0.56,0],</v>
-      </c>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior'</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>319</v>
       </c>
@@ -18118,16 +18993,27 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A9," ","_") &amp; "' : [" &amp; (F9*-1) &amp; "," &amp; (E9*-1) &amp; "," &amp;(D9*-1)&amp; "," &amp; G9 &amp; "," &amp; H9 &amp; "],"</f>
+        <v>'novice' : [-1,-1,0,2,1],</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A9," ","_")  &amp; "_pct' : [" &amp; ROUND(((F9/B9)*-1),2) &amp; "," &amp; ROUND(((E9/B9)*-1),2) &amp; "," &amp; ROUND(((D9/B9)*-1),2)  &amp; "," &amp; ROUND((G9/B9),2) &amp; "," &amp; ROUND((H9/B9),2) &amp; "],"</f>
+        <v>'novice_pct' : [-0.2,-0.2,0,0.4,0.2],</v>
+      </c>
+      <c r="K9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'novice' : [-1,-1,0,2,1],</v>
-      </c>
-      <c r="J9" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
+      </c>
+      <c r="L9" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'novice_pct' : [-0.2,-0.2,0,0.4,0.2],</v>
-      </c>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice'</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -18136,26 +19022,37 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="b">
-        <f t="shared" ref="E10:H10" si="4">SUM(E7:E9)=E2</f>
+        <f t="shared" ref="E10:H10" si="6">SUM(E7:E9)=E2</f>
         <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
@@ -18182,16 +19079,27 @@
         <v>0</v>
       </c>
       <c r="I11" s="7" t="str">
+        <f t="shared" ref="I11" si="7">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <v>'current' : [-2,-3,-1,6,0],</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A11," ","_")  &amp; "_pct' : [" &amp; ROUND(((F11/B11)*-1),2) &amp; "," &amp; ROUND(((E11/B11)*-1),2) &amp; "," &amp; ROUND(((D11/B11)*-1),2)  &amp; "," &amp; ROUND((G11/B11),2) &amp; "," &amp; ROUND((H11/B11),2) &amp; "],"</f>
+        <v>'current_pct' : [-0.17,-0.25,-0.08,0.5,0],</v>
+      </c>
+      <c r="K11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'current' : [-2,-3,-1,6,0],</v>
-      </c>
-      <c r="J11" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'current_pct' : [-0.17,-0.25,-0.08,0.5,0],</v>
-      </c>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -18218,16 +19126,27 @@
         <v>1</v>
       </c>
       <c r="I12" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A12," ","_") &amp; "' : [" &amp; (F12*-1) &amp; "," &amp; (E12*-1) &amp; "," &amp;(D12*-1)&amp; "," &amp; G12 &amp; "," &amp; H12 &amp; "],"</f>
+        <v>'past' : [-1,-4,-3,9,1],</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A12," ","_")  &amp; "_pct' : [" &amp; ROUND(((F12/B12)*-1),2) &amp; "," &amp; ROUND(((E12/B12)*-1),2) &amp; "," &amp; ROUND(((D12/B12)*-1),2)  &amp; "," &amp; ROUND((G12/B12),2) &amp; "," &amp; ROUND((H12/B12),2) &amp; "],"</f>
+        <v>'past_pct' : [-0.06,-0.22,-0.17,0.5,0.06],</v>
+      </c>
+      <c r="K12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'past' : [-1,-4,-3,9,1],</v>
-      </c>
-      <c r="J12" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx]</v>
+      </c>
+      <c r="L12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'past_pct' : [-0.06,-0.22,-0.17,0.5,0.06],</v>
-      </c>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past'</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -18236,26 +19155,37 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="5">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="8">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table'</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>326</v>
       </c>
@@ -18282,15 +19212,27 @@
         <v>0</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14:I15" si="6">"'"&amp;A14 &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
-        <v>'decision table' : [-2,-6,-4,6,0],</v>
+        <f t="shared" ref="I14" si="9">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <v>'decision_table' : [-2,-6,-4,6,0],</v>
       </c>
       <c r="J14" s="7" t="str">
-        <f t="shared" ref="J14:J15" si="7">"'" &amp; A14 &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
-        <v>'decision table_pct' : [-0.11,-0.33,-0.22,0.33,0],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A14," ","_")  &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
+        <v>'decision_table_pct' : [-0.11,-0.33,-0.22,0.33,0],</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table'</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>327</v>
       </c>
@@ -18317,37 +19259,61 @@
         <v>1</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f>"'"&amp;SUBSTITUTE(A15," ","_") &amp; "' : [" &amp; (F15*-1) &amp; "," &amp; (E15*-1) &amp; "," &amp;(D15*-1)&amp; "," &amp; G15 &amp; "," &amp; H15 &amp; "],"</f>
         <v>'spreadsheet' : [-1,-1,0,9,1],</v>
       </c>
       <c r="J15" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f>"'" &amp; SUBSTITUTE(A15," ","_")  &amp; "_pct' : [" &amp; ROUND(((F15/B15)*-1),2) &amp; "," &amp; ROUND(((E15/B15)*-1),2) &amp; "," &amp; ROUND(((D15/B15)*-1),2)  &amp; "," &amp; ROUND((G15/B15),2) &amp; "," &amp; ROUND((H15/B15),2) &amp; "],"</f>
         <v>'spreadsheet_pct' : [-0.08,-0.08,0,0.75,0.08],</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx]</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet'</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D16" s="7" t="b">
         <f>SUM(D14:D15)=D$2</f>
         <v>1</v>
       </c>
       <c r="E16" s="7" t="b">
-        <f t="shared" ref="E16:H16" si="8">SUM(E14:E15)=E$2</f>
+        <f t="shared" ref="E16:H16" si="10">SUM(E14:E15)=E$2</f>
         <v>1</v>
       </c>
       <c r="F16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H16" s="7" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M16" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>328</v>
       </c>
@@ -18374,15 +19340,27 @@
         <v>1</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" ref="I17:I18" si="9">"'"&amp;A17 &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
-        <v>'ruleset 1' : [-1,-5,-4,7,1],</v>
+        <f t="shared" ref="I17" si="11">"'"&amp;SUBSTITUTE(A17," ","_") &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
+        <v>'ruleset_1' : [-1,-5,-4,7,1],</v>
       </c>
       <c r="J17" s="7" t="str">
-        <f t="shared" ref="J17:J18" si="10">"'" &amp; A17 &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
-        <v>'ruleset 1_pct' : [-0.06,-0.28,-0.22,0.39,0.06],</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A17," ","_")  &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
+        <v>'ruleset_1_pct' : [-0.06,-0.28,-0.22,0.39,0.06],</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f>IF(ISBLANK(A17),K18,K18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f t="shared" ref="L17" si="12">IF(ISBLANK(A17),L18,L18&amp;",'"&amp; A17 &amp;"'")</f>
+        <v>['ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f>IF(ISBLANK(A17),M18,M18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"[xx]")</f>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>329</v>
       </c>
@@ -18409,35 +19387,55 @@
         <v>0</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>'ruleset 2' : [-2,-2,0,8,0],</v>
+        <f>"'"&amp;SUBSTITUTE(A18," ","_") &amp; "' : [" &amp; (F18*-1) &amp; "," &amp; (E18*-1) &amp; "," &amp;(D18*-1)&amp; "," &amp; G18 &amp; "," &amp; H18 &amp; "],"</f>
+        <v>'ruleset_2' : [-2,-2,0,8,0],</v>
       </c>
       <c r="J18" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>'ruleset 2_pct' : [-0.17,-0.17,0,0.67,0],</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A18," ","_")  &amp; "_pct' : [" &amp; ROUND(((F18/B18)*-1),2) &amp; "," &amp; ROUND(((E18/B18)*-1),2) &amp; "," &amp; ROUND(((D18/B18)*-1),2)  &amp; "," &amp; ROUND((G18/B18),2) &amp; "," &amp; ROUND((H18/B18),2) &amp; "],"</f>
+        <v>'ruleset_2_pct' : [-0.17,-0.17,0,0.67,0],</v>
+      </c>
+      <c r="K18" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A18," ","_") &amp;"_pct[xx]"</f>
+        <v>[df.ruleset_2_pct[xx]</v>
+      </c>
+      <c r="L18" s="7" t="str">
+        <f>"['"&amp; A18&amp;"'"</f>
+        <v>['ruleset 2'</v>
+      </c>
+      <c r="M18" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A18," ","_") &amp;"[xx]"</f>
+        <v>[df.ruleset_2[xx]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D19" s="7" t="b">
         <f>SUM(D17:D18)=D$2</f>
         <v>1</v>
       </c>
       <c r="E19" s="7" t="b">
-        <f t="shared" ref="E19:H19" si="11">SUM(E17:E18)=E$2</f>
+        <f t="shared" ref="E19:H19" si="13">SUM(E17:E18)=E$2</f>
         <v>1</v>
       </c>
       <c r="F19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="G19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="H19" s="7" t="b">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18446,15 +19444,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1B907A-BDC5-43B2-8A49-E12C94F4DB80}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J19"/>
+      <selection activeCell="K2" sqref="K2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>315</v>
@@ -18480,7 +19478,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>311</v>
       </c>
@@ -18507,15 +19505,27 @@
         <v>1</v>
       </c>
       <c r="I2" s="7" t="str">
-        <f>"'"&amp;A2 &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A2," ","_") &amp; "' : [" &amp; (F2*-1) &amp; "," &amp; (E2*-1) &amp; "," &amp;(D2*-1)&amp; "," &amp; G2 &amp; "," &amp; H2 &amp; "],"</f>
         <v>'total' : [-9,-10,-2,7,1],</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>"'" &amp; A2 &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A2," ","_")  &amp; "_pct' : [" &amp; ROUND(((F2/B2)*-1),2) &amp; "," &amp; ROUND(((E2/B2)*-1),2) &amp; "," &amp; ROUND(((D2/B2)*-1),2)  &amp; "," &amp; ROUND((G2/B2),2) &amp; "," &amp; ROUND((H2/B2),2) &amp; "],"</f>
         <v>'total_pct' : [-0.31,-0.34,-0.07,0.24,0.03],</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="7" t="str">
+        <f>IF(ISBLANK(A2),K3,K3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"_pct[xx]]")</f>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx],df.total_pct[xx]]</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>IF(ISBLANK(A2),L3,L3&amp;",'"&amp; A2 &amp;"']")</f>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic','total']</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>IF(ISBLANK(A2),M3,M3&amp;",df."&amp; SUBSTITUTE(A2," ","_") &amp;"[xx]]")</f>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx],df.total[xx]]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -18526,8 +19536,20 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="str">
+        <f t="shared" ref="K3:K16" si="1">IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="shared" ref="L3:L16" si="2">IF(ISBLANK(A3),L4,L4&amp;",'"&amp; A3 &amp;"'")</f>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M3" s="7" t="str">
+        <f t="shared" ref="M3:M16" si="3">IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>312</v>
       </c>
@@ -18554,15 +19576,27 @@
         <v>0</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I12" si="1">"'"&amp;A4 &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
+        <f>"'"&amp;SUBSTITUTE(A4," ","_") &amp; "' : [" &amp; (F4*-1) &amp; "," &amp; (E4*-1) &amp; "," &amp;(D4*-1)&amp; "," &amp; G4 &amp; "," &amp; H4 &amp; "],"</f>
         <v>'academic' : [-4,-2,-1,3,0],</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f t="shared" ref="J4:J13" si="2">"'" &amp; A4 &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
+        <f>"'" &amp; SUBSTITUTE(A4," ","_")  &amp; "_pct' : [" &amp; ROUND(((F4/B4)*-1),2) &amp; "," &amp; ROUND(((E4/B4)*-1),2) &amp; "," &amp; ROUND(((D4/B4)*-1),2)  &amp; "," &amp; ROUND((G4/B4),2) &amp; "," &amp; ROUND((H4/B4),2) &amp; "],"</f>
         <v>'academic_pct' : [-0.4,-0.2,-0.1,0.3,0],</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
+      </c>
+      <c r="L4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
+      </c>
+      <c r="M4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>313</v>
       </c>
@@ -18589,15 +19623,27 @@
         <v>1</v>
       </c>
       <c r="I5" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A5," ","_") &amp; "' : [" &amp; (F5*-1) &amp; "," &amp; (E5*-1) &amp; "," &amp;(D5*-1)&amp; "," &amp; G5 &amp; "," &amp; H5 &amp; "],"</f>
+        <v>'practicioner' : [-5,-8,-1,4,1],</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A5," ","_")  &amp; "_pct' : [" &amp; ROUND(((F5/B5)*-1),2) &amp; "," &amp; ROUND(((E5/B5)*-1),2) &amp; "," &amp; ROUND(((D5/B5)*-1),2)  &amp; "," &amp; ROUND((G5/B5),2) &amp; "," &amp; ROUND((H5/B5),2) &amp; "],"</f>
+        <v>'practicioner_pct' : [-0.26,-0.42,-0.05,0.21,0.05],</v>
+      </c>
+      <c r="K5" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'practicioner' : [-5,-8,-1,4,1],</v>
-      </c>
-      <c r="J5" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'practicioner_pct' : [-0.26,-0.42,-0.05,0.21,0.05],</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner'</v>
+      </c>
+      <c r="M5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -18606,25 +19652,37 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="3">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="4">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H6" s="7" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>317</v>
       </c>
@@ -18651,15 +19709,27 @@
         <v>1</v>
       </c>
       <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7" si="5">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <v>'expert' : [-3,-4,0,1,1],</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A7," ","_")  &amp; "_pct' : [" &amp; ROUND(((F7/B7)*-1),2) &amp; "," &amp; ROUND(((E7/B7)*-1),2) &amp; "," &amp; ROUND(((D7/B7)*-1),2)  &amp; "," &amp; ROUND((G7/B7),2) &amp; "," &amp; ROUND((H7/B7),2) &amp; "],"</f>
+        <v>'expert_pct' : [-0.33,-0.44,0,0.11,0.11],</v>
+      </c>
+      <c r="K7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'expert' : [-3,-4,0,1,1],</v>
-      </c>
-      <c r="J7" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
+      </c>
+      <c r="L7" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'expert_pct' : [-0.33,-0.44,0,0.11,0.11],</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
+      </c>
+      <c r="M7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>318</v>
       </c>
@@ -18686,15 +19756,27 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A8," ","_") &amp; "' : [" &amp; (F8*-1) &amp; "," &amp; (E8*-1) &amp; "," &amp;(D8*-1)&amp; "," &amp; G8 &amp; "," &amp; H8 &amp; "],"</f>
+        <v>'senior' : [-4,-4,-2,5,0],</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A8," ","_")  &amp; "_pct' : [" &amp; ROUND(((F8/B8)*-1),2) &amp; "," &amp; ROUND(((E8/B8)*-1),2) &amp; "," &amp; ROUND(((D8/B8)*-1),2)  &amp; "," &amp; ROUND((G8/B8),2) &amp; "," &amp; ROUND((H8/B8),2) &amp; "],"</f>
+        <v>'senior_pct' : [-0.27,-0.27,-0.13,0.33,0],</v>
+      </c>
+      <c r="K8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'senior' : [-4,-4,-2,5,0],</v>
-      </c>
-      <c r="J8" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
+      </c>
+      <c r="L8" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'senior_pct' : [-0.27,-0.27,-0.13,0.33,0],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior'</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>319</v>
       </c>
@@ -18721,15 +19803,27 @@
         <v>0</v>
       </c>
       <c r="I9" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A9," ","_") &amp; "' : [" &amp; (F9*-1) &amp; "," &amp; (E9*-1) &amp; "," &amp;(D9*-1)&amp; "," &amp; G9 &amp; "," &amp; H9 &amp; "],"</f>
+        <v>'novice' : [-2,-2,0,1,0],</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A9," ","_")  &amp; "_pct' : [" &amp; ROUND(((F9/B9)*-1),2) &amp; "," &amp; ROUND(((E9/B9)*-1),2) &amp; "," &amp; ROUND(((D9/B9)*-1),2)  &amp; "," &amp; ROUND((G9/B9),2) &amp; "," &amp; ROUND((H9/B9),2) &amp; "],"</f>
+        <v>'novice_pct' : [-0.4,-0.4,0,0.2,0],</v>
+      </c>
+      <c r="K9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'novice' : [-2,-2,0,1,0],</v>
-      </c>
-      <c r="J9" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
+      </c>
+      <c r="L9" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'novice_pct' : [-0.4,-0.4,0,0.2,0],</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice'</v>
+      </c>
+      <c r="M9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -18738,25 +19832,37 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="b">
-        <f t="shared" ref="E10:H10" si="4">SUM(E7:E9)=E2</f>
+        <f t="shared" ref="E10:H10" si="6">SUM(E7:E9)=E2</f>
         <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>320</v>
       </c>
@@ -18783,15 +19889,27 @@
         <v>0</v>
       </c>
       <c r="I11" s="7" t="str">
+        <f t="shared" ref="I11" si="7">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <v>'current' : [-2,-6,0,3,0],</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A11," ","_")  &amp; "_pct' : [" &amp; ROUND(((F11/B11)*-1),2) &amp; "," &amp; ROUND(((E11/B11)*-1),2) &amp; "," &amp; ROUND(((D11/B11)*-1),2)  &amp; "," &amp; ROUND((G11/B11),2) &amp; "," &amp; ROUND((H11/B11),2) &amp; "],"</f>
+        <v>'current_pct' : [-0.18,-0.55,0,0.27,0],</v>
+      </c>
+      <c r="K11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'current' : [-2,-6,0,3,0],</v>
-      </c>
-      <c r="J11" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
+      </c>
+      <c r="L11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'current_pct' : [-0.18,-0.55,0,0.27,0],</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
+      </c>
+      <c r="M11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -18818,15 +19936,27 @@
         <v>1</v>
       </c>
       <c r="I12" s="7" t="str">
+        <f>"'"&amp;SUBSTITUTE(A12," ","_") &amp; "' : [" &amp; (F12*-1) &amp; "," &amp; (E12*-1) &amp; "," &amp;(D12*-1)&amp; "," &amp; G12 &amp; "," &amp; H12 &amp; "],"</f>
+        <v>'past' : [-7,-4,-2,4,1],</v>
+      </c>
+      <c r="J12" s="7" t="str">
+        <f>"'" &amp; SUBSTITUTE(A12," ","_")  &amp; "_pct' : [" &amp; ROUND(((F12/B12)*-1),2) &amp; "," &amp; ROUND(((E12/B12)*-1),2) &amp; "," &amp; ROUND(((D12/B12)*-1),2)  &amp; "," &amp; ROUND((G12/B12),2) &amp; "," &amp; ROUND((H12/B12),2) &amp; "],"</f>
+        <v>'past_pct' : [-0.39,-0.22,-0.11,0.22,0.06],</v>
+      </c>
+      <c r="K12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>'past' : [-7,-4,-2,4,1],</v>
-      </c>
-      <c r="J12" s="7" t="str">
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx]</v>
+      </c>
+      <c r="L12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>'past_pct' : [-0.39,-0.22,-0.11,0.22,0.06],</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table','past'</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -18835,25 +19965,37 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="5">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="8">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
+      </c>
+      <c r="L13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table'</v>
+      </c>
+      <c r="M13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>326</v>
       </c>
@@ -18880,15 +20022,27 @@
         <v>1</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14:I15" si="6">"'"&amp;A14 &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
-        <v>'decision table' : [-3,-7,-2,5,1],</v>
+        <f t="shared" ref="I14" si="9">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <v>'decision_table' : [-3,-7,-2,5,1],</v>
       </c>
       <c r="J14" s="7" t="str">
-        <f t="shared" ref="J14:J15" si="7">"'" &amp; A14 &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
-        <v>'decision table_pct' : [-0.17,-0.39,-0.11,0.28,0.06],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A14," ","_")  &amp; "_pct' : [" &amp; ROUND(((F14/B14)*-1),2) &amp; "," &amp; ROUND(((E14/B14)*-1),2) &amp; "," &amp; ROUND(((D14/B14)*-1),2)  &amp; "," &amp; ROUND((G14/B14),2) &amp; "," &amp; ROUND((H14/B14),2) &amp; "],"</f>
+        <v>'decision_table_pct' : [-0.17,-0.39,-0.11,0.28,0.06],</v>
+      </c>
+      <c r="K14" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
+      </c>
+      <c r="L14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet','decision table'</v>
+      </c>
+      <c r="M14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>327</v>
       </c>
@@ -18915,15 +20069,27 @@
         <v>0</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f>"'"&amp;SUBSTITUTE(A15," ","_") &amp; "' : [" &amp; (F15*-1) &amp; "," &amp; (E15*-1) &amp; "," &amp;(D15*-1)&amp; "," &amp; G15 &amp; "," &amp; H15 &amp; "],"</f>
         <v>'spreadsheet' : [-6,-3,0,2,0],</v>
       </c>
       <c r="J15" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f>"'" &amp; SUBSTITUTE(A15," ","_")  &amp; "_pct' : [" &amp; ROUND(((F15/B15)*-1),2) &amp; "," &amp; ROUND(((E15/B15)*-1),2) &amp; "," &amp; ROUND(((D15/B15)*-1),2)  &amp; "," &amp; ROUND((G15/B15),2) &amp; "," &amp; ROUND((H15/B15),2) &amp; "],"</f>
         <v>'spreadsheet_pct' : [-0.55,-0.27,0,0.18,0],</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx]</v>
+      </c>
+      <c r="L15" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1','spreadsheet'</v>
+      </c>
+      <c r="M15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -18932,25 +20098,37 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="b">
-        <f t="shared" ref="E16:H16" si="8">SUM(E14:E15)=E$2</f>
+        <f t="shared" ref="E16:H16" si="10">SUM(E14:E15)=E$2</f>
         <v>1</v>
       </c>
       <c r="F16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L16" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>['ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M16" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>328</v>
       </c>
@@ -18977,15 +20155,27 @@
         <v>1</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" ref="I17:I18" si="9">"'"&amp;A17 &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
-        <v>'ruleset 1' : [-2,-4,-1,3,1],</v>
+        <f t="shared" ref="I17" si="11">"'"&amp;SUBSTITUTE(A17," ","_") &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
+        <v>'ruleset_1' : [-2,-4,-1,3,1],</v>
       </c>
       <c r="J17" s="7" t="str">
-        <f t="shared" ref="J17:J18" si="10">"'" &amp; A17 &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
-        <v>'ruleset 1_pct' : [-0.18,-0.36,-0.09,0.27,0.09],</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A17," ","_")  &amp; "_pct' : [" &amp; ROUND(((F17/B17)*-1),2) &amp; "," &amp; ROUND(((E17/B17)*-1),2) &amp; "," &amp; ROUND(((D17/B17)*-1),2)  &amp; "," &amp; ROUND((G17/B17),2) &amp; "," &amp; ROUND((H17/B17),2) &amp; "],"</f>
+        <v>'ruleset_1_pct' : [-0.18,-0.36,-0.09,0.27,0.09],</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f>IF(ISBLANK(A17),K18,K18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"_pct[xx]")</f>
+        <v>[df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f t="shared" ref="L17" si="12">IF(ISBLANK(A17),L18,L18&amp;",'"&amp; A17 &amp;"'")</f>
+        <v>['ruleset 2','ruleset 1'</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f>IF(ISBLANK(A17),M18,M18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"[xx]")</f>
+        <v>[df.ruleset_2[xx],df.ruleset_1[xx]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>329</v>
       </c>
@@ -19012,15 +20202,27 @@
         <v>0</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>'ruleset 2' : [-7,-6,-1,4,0],</v>
+        <f>"'"&amp;SUBSTITUTE(A18," ","_") &amp; "' : [" &amp; (F18*-1) &amp; "," &amp; (E18*-1) &amp; "," &amp;(D18*-1)&amp; "," &amp; G18 &amp; "," &amp; H18 &amp; "],"</f>
+        <v>'ruleset_2' : [-7,-6,-1,4,0],</v>
       </c>
       <c r="J18" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>'ruleset 2_pct' : [-0.39,-0.33,-0.06,0.22,0],</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+        <f>"'" &amp; SUBSTITUTE(A18," ","_")  &amp; "_pct' : [" &amp; ROUND(((F18/B18)*-1),2) &amp; "," &amp; ROUND(((E18/B18)*-1),2) &amp; "," &amp; ROUND(((D18/B18)*-1),2)  &amp; "," &amp; ROUND((G18/B18),2) &amp; "," &amp; ROUND((H18/B18),2) &amp; "],"</f>
+        <v>'ruleset_2_pct' : [-0.39,-0.33,-0.06,0.22,0],</v>
+      </c>
+      <c r="K18" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A18," ","_") &amp;"_pct[xx]"</f>
+        <v>[df.ruleset_2_pct[xx]</v>
+      </c>
+      <c r="L18" s="7" t="str">
+        <f>"['"&amp; A18&amp;"'"</f>
+        <v>['ruleset 2'</v>
+      </c>
+      <c r="M18" s="7" t="str">
+        <f>"[df."&amp; SUBSTITUTE(A18," ","_") &amp;"[xx]"</f>
+        <v>[df.ruleset_2[xx]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -19029,23 +20231,31 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="b">
-        <f t="shared" ref="E19:H19" si="11">SUM(E17:E18)=E$2</f>
+        <f t="shared" ref="E19:H19" si="13">SUM(E17:E18)=E$2</f>
         <v>1</v>
       </c>
       <c r="F19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="G19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="H19" s="7" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lost of stuff to back up
</commit_message>
<xml_diff>
--- a/survey analysis.xlsx
+++ b/survey analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Thesis2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B2795C-241F-41DC-A888-1A9A44B65415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164EB28E-365B-4382-9FE0-DDBBDAC0319B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23520" yWindow="-16665" windowWidth="28440" windowHeight="11820" tabRatio="705" firstSheet="2" activeTab="10" xr2:uid="{CF2921A5-C80B-4877-A0CE-2F57B984B9AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="705" activeTab="9" xr2:uid="{CF2921A5-C80B-4877-A0CE-2F57B984B9AC}"/>
   </bookViews>
   <sheets>
     <sheet name="deliveries" sheetId="1" r:id="rId1"/>
@@ -5600,6 +5600,203 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9EB97D2-B220-420F-9482-6B2082BF4693}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I9:J25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="44">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="31"/>
+    <field x="27"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="5" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Respondent ID" fld="0" subtotal="count" baseField="9" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{349D25D2-486B-45F2-8B43-2C24FC525FFD}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E11:F16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="29">
@@ -5697,7 +5894,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5624DE0F-B479-4E43-A407-7F4A6D86F76C}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="44">
@@ -5922,203 +6119,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Respondent ID" fld="0" subtotal="count" baseField="6" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9EB97D2-B220-420F-9482-6B2082BF4693}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I9:J25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="44">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="31"/>
-    <field x="27"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="5" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Respondent ID" fld="0" subtotal="count" baseField="9" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -6819,8 +6819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7F3328-AE59-4804-B9D0-19F41318D13C}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" activeCellId="1" sqref="K15:M15 J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7526,7 +7526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E89FD6-A5B3-49FA-9795-07F4C25BE734}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -11734,8 +11734,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AR44" sqref="AR2:AR44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11898,7 +11898,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>12911218992</v>
       </c>
@@ -12139,7 +12139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>12900124256</v>
       </c>
@@ -12324,7 +12324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>12897741246</v>
       </c>
@@ -12447,7 +12447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>12897615131</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>12897591538</v>
       </c>
@@ -12693,7 +12693,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>12894927604</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>12889889233</v>
       </c>
@@ -15285,7 +15285,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>12911214937</v>
       </c>
@@ -15405,7 +15405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>12911152204</v>
       </c>
@@ -15595,7 +15595,7 @@
       </c>
       <c r="AK37" s="7"/>
     </row>
-    <row r="38" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>12903401040</v>
       </c>
@@ -15839,7 +15839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>12897594233</v>
       </c>
@@ -15971,7 +15971,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>12894836898</v>
       </c>
@@ -16094,7 +16094,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>12894677080</v>
       </c>
@@ -16217,7 +16217,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>12892108857</v>
       </c>
@@ -16342,12 +16342,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AS44" xr:uid="{B2878579-3EAB-4A8E-AC2E-5F0A9ACDF432}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="B"/>
-        <filter val="C"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="TRUE"/>
@@ -16870,8 +16864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C22359-5314-43E8-AF1A-50A8F1058A66}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16967,7 +16961,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="str">
-        <f>IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" ref="K3:K20" si="1">IF(ISBLANK(A3),K4,K4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"_pct[xx]")</f>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
       </c>
       <c r="L3" s="7" t="str">
@@ -16975,7 +16969,7 @@
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
       </c>
       <c r="M3" s="7" t="str">
-        <f>IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
+        <f t="shared" ref="M3:M20" si="2">IF(ISBLANK(A3),M4,M4&amp;",df."&amp; SUBSTITUTE(A3," ","_") &amp;"[xx]")</f>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
       </c>
     </row>
@@ -17014,15 +17008,15 @@
         <v>'academic_pct' : [-0.4,-0.3,0,0.1,0.2],</v>
       </c>
       <c r="K4" s="7" t="str">
-        <f>IF(ISBLANK(A4),K5,K5&amp;",df."&amp; SUBSTITUTE(A4," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx],df.academic_pct[xx]</v>
       </c>
       <c r="L4" s="7" t="str">
-        <f t="shared" ref="L4:L20" si="1">IF(ISBLANK(A4),L5,L5&amp;",'"&amp; A4 &amp;"'")</f>
+        <f t="shared" ref="L4:L20" si="3">IF(ISBLANK(A4),L5,L5&amp;",'"&amp; A4 &amp;"'")</f>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner','academic'</v>
       </c>
       <c r="M4" s="7" t="str">
-        <f>IF(ISBLANK(A4),M5,M5&amp;",df."&amp; SUBSTITUTE(A4," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx],df.academic[xx]</v>
       </c>
     </row>
@@ -17061,15 +17055,15 @@
         <v>'practicioner_pct' : [-0.3,-0.1,-0.05,0.3,0.25],</v>
       </c>
       <c r="K5" s="7" t="str">
-        <f>IF(ISBLANK(A5),K6,K6&amp;",df."&amp; SUBSTITUTE(A5," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx],df.practicioner_pct[xx]</v>
       </c>
       <c r="L5" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert','practicioner'</v>
       </c>
       <c r="M5" s="7" t="str">
-        <f>IF(ISBLANK(A5),M6,M6&amp;",df."&amp; SUBSTITUTE(A5," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx],df.practicioner[xx]</v>
       </c>
     </row>
@@ -17082,33 +17076,33 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="b">
-        <f t="shared" ref="E6:H6" si="2">SUM(E4:E5)=E2</f>
+        <f t="shared" ref="E6:H6" si="4">SUM(E4:E5)=E2</f>
         <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6" s="7" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H6" s="7" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="str">
-        <f>IF(ISBLANK(A6),K7,K7&amp;",df."&amp; SUBSTITUTE(A6," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
       </c>
       <c r="L6" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
       </c>
       <c r="M6" s="7" t="str">
-        <f>IF(ISBLANK(A6),M7,M7&amp;",df."&amp; SUBSTITUTE(A6," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
       </c>
     </row>
@@ -17139,7 +17133,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f t="shared" ref="I7" si="3">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
+        <f t="shared" ref="I7" si="5">"'"&amp;SUBSTITUTE(A7," ","_") &amp; "' : [" &amp; (F7*-1) &amp; "," &amp; (E7*-1) &amp; "," &amp;(D7*-1)&amp; "," &amp; G7 &amp; "," &amp; H7 &amp; "],"</f>
         <v>'expert' : [-3,-1,-1,2,2],</v>
       </c>
       <c r="J7" s="7" t="str">
@@ -17147,15 +17141,15 @@
         <v>'expert_pct' : [-0.33,-0.11,-0.11,0.22,0.22],</v>
       </c>
       <c r="K7" s="7" t="str">
-        <f>IF(ISBLANK(A7),K8,K8&amp;",df."&amp; SUBSTITUTE(A7," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx],df.expert_pct[xx]</v>
       </c>
       <c r="L7" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior','expert'</v>
       </c>
       <c r="M7" s="7" t="str">
-        <f>IF(ISBLANK(A7),M8,M8&amp;",df."&amp; SUBSTITUTE(A7," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx],df.expert[xx]</v>
       </c>
     </row>
@@ -17194,15 +17188,15 @@
         <v>'senior_pct' : [-0.31,-0.13,0,0.31,0.25],</v>
       </c>
       <c r="K8" s="7" t="str">
-        <f>IF(ISBLANK(A8),K9,K9&amp;",df."&amp; SUBSTITUTE(A8," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx],df.senior_pct[xx]</v>
       </c>
       <c r="L8" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice','senior'</v>
       </c>
       <c r="M8" s="7" t="str">
-        <f>IF(ISBLANK(A8),M9,M9&amp;",df."&amp; SUBSTITUTE(A8," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx],df.senior[xx]</v>
       </c>
     </row>
@@ -17241,15 +17235,15 @@
         <v>'novice_pct' : [-0.4,-0.4,0,0,0.2],</v>
       </c>
       <c r="K9" s="7" t="str">
-        <f>IF(ISBLANK(A9),K10,K10&amp;",df."&amp; SUBSTITUTE(A9," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx],df.novice_pct[xx]</v>
       </c>
       <c r="L9" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current','novice'</v>
       </c>
       <c r="M9" s="7" t="str">
-        <f>IF(ISBLANK(A9),M10,M10&amp;",df."&amp; SUBSTITUTE(A9," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx],df.novice[xx]</v>
       </c>
     </row>
@@ -17262,33 +17256,33 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="b">
-        <f t="shared" ref="E10:H10" si="4">SUM(E7:E9)=E2</f>
+        <f t="shared" ref="E10:H10" si="6">SUM(E7:E9)=E2</f>
         <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H10" s="7" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7" t="str">
-        <f>IF(ISBLANK(A10),K11,K11&amp;",df."&amp; SUBSTITUTE(A10," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
       </c>
       <c r="L10" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
       </c>
       <c r="M10" s="7" t="str">
-        <f>IF(ISBLANK(A10),M11,M11&amp;",df."&amp; SUBSTITUTE(A10," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
       </c>
     </row>
@@ -17319,7 +17313,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="7" t="str">
-        <f t="shared" ref="I11" si="5">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
+        <f t="shared" ref="I11" si="7">"'"&amp;SUBSTITUTE(A11," ","_") &amp; "' : [" &amp; (F11*-1) &amp; "," &amp; (E11*-1) &amp; "," &amp;(D11*-1)&amp; "," &amp; G11 &amp; "," &amp; H11 &amp; "],"</f>
         <v>'current' : [-5,-2,-1,2,2],</v>
       </c>
       <c r="J11" s="7" t="str">
@@ -17327,15 +17321,15 @@
         <v>'current_pct' : [-0.42,-0.17,-0.08,0.17,0.17],</v>
       </c>
       <c r="K11" s="7" t="str">
-        <f>IF(ISBLANK(A11),K12,K12&amp;",df."&amp; SUBSTITUTE(A11," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx],df.current_pct[xx]</v>
       </c>
       <c r="L11" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past','current'</v>
       </c>
       <c r="M11" s="7" t="str">
-        <f>IF(ISBLANK(A11),M12,M12&amp;",df."&amp; SUBSTITUTE(A11," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx],df.current[xx]</v>
       </c>
     </row>
@@ -17374,15 +17368,15 @@
         <v>'past_pct' : [-0.28,-0.17,0,0.28,0.28],</v>
       </c>
       <c r="K12" s="7" t="str">
-        <f>IF(ISBLANK(A12),K13,K13&amp;",df."&amp; SUBSTITUTE(A12," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx],df.past_pct[xx]</v>
       </c>
       <c r="L12" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table','past'</v>
       </c>
       <c r="M12" s="7" t="str">
-        <f>IF(ISBLANK(A12),M13,M13&amp;",df."&amp; SUBSTITUTE(A12," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx],df.past[xx]</v>
       </c>
     </row>
@@ -17395,33 +17389,33 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="b">
-        <f t="shared" ref="E13:H13" si="6">SUM(E11:E12)=E2</f>
+        <f t="shared" ref="E13:H13" si="8">SUM(E11:E12)=E2</f>
         <v>1</v>
       </c>
       <c r="F13" s="7" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G13" s="7" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H13" s="7" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7" t="str">
-        <f>IF(ISBLANK(A13),K14,K14&amp;",df."&amp; SUBSTITUTE(A13," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
       </c>
       <c r="L13" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table'</v>
       </c>
       <c r="M13" s="7" t="str">
-        <f>IF(ISBLANK(A13),M14,M14&amp;",df."&amp; SUBSTITUTE(A13," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
       </c>
     </row>
@@ -17452,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" ref="I14" si="7">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
+        <f t="shared" ref="I14" si="9">"'"&amp;SUBSTITUTE(A14," ","_") &amp; "' : [" &amp; (F14*-1) &amp; "," &amp; (E14*-1) &amp; "," &amp;(D14*-1)&amp; "," &amp; G14 &amp; "," &amp; H14 &amp; "],"</f>
         <v>'decision_table' : [-4,-5,0,2,1],</v>
       </c>
       <c r="J14" s="7" t="str">
@@ -17460,15 +17454,15 @@
         <v>'decision_table_pct' : [-0.33,-0.42,0,0.17,0.08],</v>
       </c>
       <c r="K14" s="7" t="str">
-        <f>IF(ISBLANK(A14),K15,K15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx],df.decision_table_pct[xx]</v>
       </c>
       <c r="L14" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet','decision table'</v>
       </c>
       <c r="M14" s="7" t="str">
-        <f>IF(ISBLANK(A14),M15,M15&amp;",df."&amp; SUBSTITUTE(A14," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx],df.decision_table[xx]</v>
       </c>
     </row>
@@ -17507,15 +17501,15 @@
         <v>'spreadsheet_pct' : [-0.33,0,-0.06,0.28,0.33],</v>
       </c>
       <c r="K15" s="7" t="str">
-        <f>IF(ISBLANK(A15),K16,K16&amp;",df."&amp; SUBSTITUTE(A15," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx],df.spreadsheet_pct[xx]</v>
       </c>
       <c r="L15" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1','spreadsheet'</v>
       </c>
       <c r="M15" s="7" t="str">
-        <f>IF(ISBLANK(A15),M16,M16&amp;",df."&amp; SUBSTITUTE(A15," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx],df.spreadsheet[xx]</v>
       </c>
     </row>
@@ -17525,31 +17519,31 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="b">
-        <f t="shared" ref="E16:H16" si="8">SUM(E14:E15)=E$2</f>
+        <f t="shared" ref="E16:H16" si="10">SUM(E14:E15)=E$2</f>
         <v>1</v>
       </c>
       <c r="F16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="G16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H16" s="7" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="K16" s="7" t="str">
-        <f>IF(ISBLANK(A16),K17,K17&amp;",df."&amp; SUBSTITUTE(A16," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
       </c>
       <c r="L16" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1'</v>
       </c>
       <c r="M16" s="7" t="str">
-        <f>IF(ISBLANK(A16),M17,M17&amp;",df."&amp; SUBSTITUTE(A16," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx]</v>
       </c>
     </row>
@@ -17580,7 +17574,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" ref="I17" si="9">"'"&amp;SUBSTITUTE(A17," ","_") &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
+        <f t="shared" ref="I17" si="11">"'"&amp;SUBSTITUTE(A17," ","_") &amp; "' : [" &amp; (F17*-1) &amp; "," &amp; (E17*-1) &amp; "," &amp;(D17*-1)&amp; "," &amp; G17 &amp; "," &amp; H17 &amp; "],"</f>
         <v>'ruleset_1' : [-6,-3,-1,5,3],</v>
       </c>
       <c r="J17" s="7" t="str">
@@ -17588,15 +17582,15 @@
         <v>'ruleset_1_pct' : [-0.33,-0.17,-0.06,0.28,0.17],</v>
       </c>
       <c r="K17" s="7" t="str">
-        <f>IF(ISBLANK(A17),K18,K18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx],df.ruleset_1_pct[xx]</v>
       </c>
       <c r="L17" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2','ruleset 1'</v>
       </c>
       <c r="M17" s="7" t="str">
-        <f>IF(ISBLANK(A17),M18,M18&amp;",df."&amp; SUBSTITUTE(A17," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx],df.ruleset_1[xx]</v>
       </c>
     </row>
@@ -17635,15 +17629,15 @@
         <v>'ruleset_2_pct' : [-0.33,-0.17,0,0.17,0.33],</v>
       </c>
       <c r="K18" s="7" t="str">
-        <f>IF(ISBLANK(A18),K19,K19&amp;",df."&amp; SUBSTITUTE(A18," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx],df.ruleset_2_pct[xx]</v>
       </c>
       <c r="L18" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection','ruleset 2'</v>
       </c>
       <c r="M18" s="7" t="str">
-        <f>IF(ISBLANK(A18),M19,M19&amp;",df."&amp; SUBSTITUTE(A18," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx],df.ruleset_2[xx]</v>
       </c>
     </row>
@@ -17654,31 +17648,31 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="b">
-        <f t="shared" ref="E19" si="10">SUM(E17:E18)=E$2</f>
+        <f t="shared" ref="E19" si="12">SUM(E17:E18)=E$2</f>
         <v>1</v>
       </c>
       <c r="F19" s="7" t="b">
-        <f t="shared" ref="F19" si="11">SUM(F17:F18)=F$2</f>
+        <f t="shared" ref="F19" si="13">SUM(F17:F18)=F$2</f>
         <v>1</v>
       </c>
       <c r="G19" s="7" t="b">
-        <f t="shared" ref="G19" si="12">SUM(G17:G18)=G$2</f>
+        <f t="shared" ref="G19" si="14">SUM(G17:G18)=G$2</f>
         <v>1</v>
       </c>
       <c r="H19" s="7" t="b">
-        <f t="shared" ref="H19" si="13">SUM(H17:H18)=H$2</f>
+        <f t="shared" ref="H19" si="15">SUM(H17:H18)=H$2</f>
         <v>1</v>
       </c>
       <c r="K19" s="7" t="str">
-        <f>IF(ISBLANK(A19),K20,K20&amp;",df."&amp; SUBSTITUTE(A19," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx]</v>
       </c>
       <c r="L19" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection'</v>
       </c>
       <c r="M19" s="7" t="str">
-        <f>IF(ISBLANK(A19),M20,M20&amp;",df."&amp; SUBSTITUTE(A19," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx]</v>
       </c>
     </row>
@@ -17709,7 +17703,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="7" t="str">
-        <f t="shared" ref="I20" si="14">"'"&amp;SUBSTITUTE(A20," ","_") &amp; "' : [" &amp; (F20*-1) &amp; "," &amp; (E20*-1) &amp; "," &amp;(D20*-1)&amp; "," &amp; G20 &amp; "," &amp; H20 &amp; "],"</f>
+        <f t="shared" ref="I20" si="16">"'"&amp;SUBSTITUTE(A20," ","_") &amp; "' : [" &amp; (F20*-1) &amp; "," &amp; (E20*-1) &amp; "," &amp;(D20*-1)&amp; "," &amp; G20 &amp; "," &amp; H20 &amp; "],"</f>
         <v>'projection' : [-6,-3,0,2,3],</v>
       </c>
       <c r="J20" s="7" t="str">
@@ -17717,15 +17711,15 @@
         <v>'projection_pct' : [-0.43,-0.21,0,0.14,0.21],</v>
       </c>
       <c r="K20" s="7" t="str">
-        <f>IF(ISBLANK(A20),K21,K21&amp;",df."&amp; SUBSTITUTE(A20," ","_") &amp;"_pct[xx]")</f>
+        <f t="shared" si="1"/>
         <v>[df.text_pct[xx],df.projection_pct[xx]</v>
       </c>
       <c r="L20" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>['text','projection'</v>
       </c>
       <c r="M20" t="str">
-        <f>IF(ISBLANK(A20),M21,M21&amp;",df."&amp; SUBSTITUTE(A20," ","_") &amp;"[xx]")</f>
+        <f t="shared" si="2"/>
         <v>[df.text[xx],df.projection[xx]</v>
       </c>
     </row>
@@ -17782,19 +17776,19 @@
         <v>1</v>
       </c>
       <c r="E22" s="7" t="b">
-        <f t="shared" ref="E22" si="15">SUM(E20:E21)=E$2</f>
+        <f t="shared" ref="E22" si="17">SUM(E20:E21)=E$2</f>
         <v>1</v>
       </c>
       <c r="F22" s="7" t="b">
-        <f t="shared" ref="F22" si="16">SUM(F20:F21)=F$2</f>
+        <f t="shared" ref="F22" si="18">SUM(F20:F21)=F$2</f>
         <v>1</v>
       </c>
       <c r="G22" s="7" t="b">
-        <f t="shared" ref="G22" si="17">SUM(G20:G21)=G$2</f>
+        <f t="shared" ref="G22" si="19">SUM(G20:G21)=G$2</f>
         <v>1</v>
       </c>
       <c r="H22" s="7" t="b">
-        <f t="shared" ref="H22" si="18">SUM(H20:H21)=H$2</f>
+        <f t="shared" ref="H22" si="20">SUM(H20:H21)=H$2</f>
         <v>1</v>
       </c>
     </row>
@@ -17808,10 +17802,13 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:M2"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="35.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
@@ -18627,7 +18624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2189D71-B2C2-470B-B11E-70CE459BF187}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:M2"/>
     </sheetView>
   </sheetViews>

</xml_diff>